<commit_message>
Finished up to 3th grade
</commit_message>
<xml_diff>
--- a/Rozklad_2zaizd.xlsx
+++ b/Rozklad_2zaizd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20730" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="20730" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="216">
   <si>
     <t>І</t>
   </si>
@@ -534,6 +534,201 @@
   </si>
   <si>
     <t>ст. викл. Мельничук В.П.</t>
+  </si>
+  <si>
+    <t>Лісова ентомологія</t>
+  </si>
+  <si>
+    <t>Недеревні ресурси</t>
+  </si>
+  <si>
+    <t>доц. Мірутенко В.В.</t>
+  </si>
+  <si>
+    <t>Технічна механіка</t>
+  </si>
+  <si>
+    <t>Грунтознавство</t>
+  </si>
+  <si>
+    <t>Технічна механіка (залік)</t>
+  </si>
+  <si>
+    <t>Генетика</t>
+  </si>
+  <si>
+    <t>Генетика (іспит)</t>
+  </si>
+  <si>
+    <t>доц. Мигаль А.В.; ст.викл. Смужаниця Я.В.</t>
+  </si>
+  <si>
+    <t>Дендрологія</t>
+  </si>
+  <si>
+    <t>Фізіологія рослин</t>
+  </si>
+  <si>
+    <t>ст. викл. Смужаниця Я.В.</t>
+  </si>
+  <si>
+    <t>Лісознавство</t>
+  </si>
+  <si>
+    <t>викл. Бубенко С.П.</t>
+  </si>
+  <si>
+    <t>Загальна гідрологія і океанологія</t>
+  </si>
+  <si>
+    <t>Палеогеографія плейстоцену</t>
+  </si>
+  <si>
+    <t>Палеогеографія плейстоцену (залік)</t>
+  </si>
+  <si>
+    <t>Загальна гідрологія і океанологія (іспит)</t>
+  </si>
+  <si>
+    <t>Методи географічних досліджень</t>
+  </si>
+  <si>
+    <t>Методи географічних досліджень (іспит)</t>
+  </si>
+  <si>
+    <t>Ландшафтознавство з основами  ландшафтної екології</t>
+  </si>
+  <si>
+    <t>викл. Корчинська Ж.М.</t>
+  </si>
+  <si>
+    <t>викл. Корчинська Ж.М., викл. Лета В.В.</t>
+  </si>
+  <si>
+    <t>Регіональна економічна і соціальна географія</t>
+  </si>
+  <si>
+    <t>ст. викл. Антонюк О.С.</t>
+  </si>
+  <si>
+    <t>Основи менеджменту та маркетингу</t>
+  </si>
+  <si>
+    <t>ст. викл. Жулканич Б.М.</t>
+  </si>
+  <si>
+    <t>Науково-дослідна робота студентів</t>
+  </si>
+  <si>
+    <t>Науково-дослідна робота студентів (залік)</t>
+  </si>
+  <si>
+    <t>Географія сільського і лісового господарства Закарпаття</t>
+  </si>
+  <si>
+    <t>Географія сільського і лісового господарства Закарпаття (іспит)</t>
+  </si>
+  <si>
+    <t>Фізична географія України (кр)</t>
+  </si>
+  <si>
+    <t>ст. викл. Яцко О.В.</t>
+  </si>
+  <si>
+    <t>ст. викл Жиган М.В.</t>
+  </si>
+  <si>
+    <t>ст.викл. Лахоцька Е.Я.</t>
+  </si>
+  <si>
+    <t>ГІС і бази даних</t>
+  </si>
+  <si>
+    <t>доц. Радиш І.П.</t>
+  </si>
+  <si>
+    <t>Математична обробка геодезичних вимірювань</t>
+  </si>
+  <si>
+    <t>ст. викл. Ничвид М.Р.</t>
+  </si>
+  <si>
+    <t>Математичні методи в землевпорядкуванні</t>
+  </si>
+  <si>
+    <t>ПРП Закарпаття</t>
+  </si>
+  <si>
+    <t>проф. Поп С.С.</t>
+  </si>
+  <si>
+    <t>ПРП Закарпаття (іспит)</t>
+  </si>
+  <si>
+    <t>Законодавчі основи землевпорядкування та кадастру</t>
+  </si>
+  <si>
+    <t>ст. викл. Марухнич Т.Б.; викл. Бубенко С.П.</t>
+  </si>
+  <si>
+    <t>Основи GPS-технологій</t>
+  </si>
+  <si>
+    <t>Інвестиційний аналіз</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Інвестиційний аналіз (залік) </t>
+  </si>
+  <si>
+    <t>доц. Славік Р.В.</t>
+  </si>
+  <si>
+    <t>Землеробство з основами рослинництва (залік)</t>
+  </si>
+  <si>
+    <t>Землеустрій</t>
+  </si>
+  <si>
+    <t>доц. Пересоляк В.Ю.</t>
+  </si>
+  <si>
+    <t>Геодезичні роботи в землеустрої</t>
+  </si>
+  <si>
+    <t>Квітникарство</t>
+  </si>
+  <si>
+    <t>Землеробство</t>
+  </si>
+  <si>
+    <t>Образотворча грамота</t>
+  </si>
+  <si>
+    <t>ст. викл. Кіс Н.Ю.</t>
+  </si>
+  <si>
+    <t>Фітопатологія</t>
+  </si>
+  <si>
+    <t>Озеленення населених місць</t>
+  </si>
+  <si>
+    <t>доц. Чепур С.С.; ст. викл. Мойш Н.І.</t>
+  </si>
+  <si>
+    <t>Декоративне луківництво</t>
+  </si>
+  <si>
+    <t>Лісові культури (кп)</t>
+  </si>
+  <si>
+    <t>Лісова селекція 3 курс</t>
+  </si>
+  <si>
+    <t>ст. викл. Задорожний А.І.</t>
+  </si>
+  <si>
+    <t>Лісова пірологія</t>
   </si>
 </sst>
 </file>
@@ -766,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -843,43 +1038,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -891,10 +1068,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1169,7 +1370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1180,10 +1381,10 @@
   <dimension ref="A1:BW90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V62" sqref="V62:W62"/>
+      <selection pane="bottomRight" activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,277 +1468,277 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="39" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="39" t="s">
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="41"/>
-      <c r="AH1" s="39" t="s">
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40"/>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40"/>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="41"/>
-      <c r="AQ1" s="39" t="s">
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
+      <c r="AO1" s="34"/>
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="40"/>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="40"/>
-      <c r="AV1" s="40"/>
-      <c r="AW1" s="40"/>
-      <c r="AX1" s="40"/>
-      <c r="AY1" s="41"/>
-      <c r="AZ1" s="39" t="s">
+      <c r="AR1" s="34"/>
+      <c r="AS1" s="34"/>
+      <c r="AT1" s="34"/>
+      <c r="AU1" s="34"/>
+      <c r="AV1" s="34"/>
+      <c r="AW1" s="34"/>
+      <c r="AX1" s="34"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="BA1" s="40"/>
-      <c r="BB1" s="40"/>
-      <c r="BC1" s="40"/>
-      <c r="BD1" s="40"/>
-      <c r="BE1" s="40"/>
-      <c r="BF1" s="40"/>
-      <c r="BG1" s="40"/>
-      <c r="BH1" s="40"/>
-      <c r="BI1" s="40"/>
-      <c r="BJ1" s="40"/>
-      <c r="BK1" s="40"/>
-      <c r="BL1" s="40"/>
-      <c r="BM1" s="40"/>
-      <c r="BN1" s="40"/>
-      <c r="BO1" s="40"/>
-      <c r="BP1" s="40"/>
-      <c r="BQ1" s="41"/>
+      <c r="BA1" s="34"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="34"/>
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="34"/>
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="34"/>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BM1" s="34"/>
+      <c r="BN1" s="34"/>
+      <c r="BO1" s="34"/>
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="35"/>
     </row>
     <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="35" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="35" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="35" t="s">
+      <c r="K2" s="28"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="37" t="s">
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="35" t="s">
+      <c r="Q2" s="28"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="35"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="35" t="s">
+      <c r="T2" s="28"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="35"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="37" t="s">
+      <c r="W2" s="28"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="35" t="s">
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="35" t="s">
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="37" t="s">
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="36"/>
-      <c r="AK2" s="35" t="s">
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AL2" s="35"/>
-      <c r="AM2" s="36"/>
-      <c r="AN2" s="35" t="s">
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" s="35"/>
-      <c r="AP2" s="38"/>
-      <c r="AQ2" s="37" t="s">
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="29"/>
+      <c r="AQ2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="AR2" s="35"/>
-      <c r="AS2" s="36"/>
-      <c r="AT2" s="35" t="s">
+      <c r="AR2" s="28"/>
+      <c r="AS2" s="31"/>
+      <c r="AT2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AU2" s="35"/>
-      <c r="AV2" s="36"/>
-      <c r="AW2" s="35" t="s">
+      <c r="AU2" s="28"/>
+      <c r="AV2" s="31"/>
+      <c r="AW2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="35"/>
-      <c r="AY2" s="38"/>
-      <c r="AZ2" s="37" t="s">
+      <c r="AX2" s="28"/>
+      <c r="AY2" s="29"/>
+      <c r="AZ2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="BA2" s="35"/>
-      <c r="BB2" s="35"/>
-      <c r="BC2" s="35"/>
-      <c r="BD2" s="35"/>
-      <c r="BE2" s="36"/>
-      <c r="BF2" s="34" t="s">
+      <c r="BA2" s="28"/>
+      <c r="BB2" s="28"/>
+      <c r="BC2" s="28"/>
+      <c r="BD2" s="28"/>
+      <c r="BE2" s="31"/>
+      <c r="BF2" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="BG2" s="35"/>
-      <c r="BH2" s="35"/>
-      <c r="BI2" s="35"/>
-      <c r="BJ2" s="35"/>
-      <c r="BK2" s="36"/>
-      <c r="BL2" s="35" t="s">
+      <c r="BG2" s="28"/>
+      <c r="BH2" s="28"/>
+      <c r="BI2" s="28"/>
+      <c r="BJ2" s="28"/>
+      <c r="BK2" s="31"/>
+      <c r="BL2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="BM2" s="35"/>
-      <c r="BN2" s="35"/>
-      <c r="BO2" s="35"/>
-      <c r="BP2" s="35"/>
-      <c r="BQ2" s="38"/>
+      <c r="BM2" s="28"/>
+      <c r="BN2" s="28"/>
+      <c r="BO2" s="28"/>
+      <c r="BP2" s="28"/>
+      <c r="BQ2" s="29"/>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="D3" s="37"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="36"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="38"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="35"/>
-      <c r="AJ3" s="36"/>
-      <c r="AK3" s="35"/>
-      <c r="AL3" s="35"/>
-      <c r="AM3" s="36"/>
-      <c r="AN3" s="35"/>
-      <c r="AO3" s="35"/>
-      <c r="AP3" s="38"/>
-      <c r="AQ3" s="37"/>
-      <c r="AR3" s="35"/>
-      <c r="AS3" s="36"/>
-      <c r="AT3" s="35"/>
-      <c r="AU3" s="35"/>
-      <c r="AV3" s="36"/>
-      <c r="AW3" s="35"/>
-      <c r="AX3" s="35"/>
-      <c r="AY3" s="38"/>
-      <c r="AZ3" s="37" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="28"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="31"/>
+      <c r="AN3" s="28"/>
+      <c r="AO3" s="28"/>
+      <c r="AP3" s="29"/>
+      <c r="AQ3" s="30"/>
+      <c r="AR3" s="28"/>
+      <c r="AS3" s="31"/>
+      <c r="AT3" s="28"/>
+      <c r="AU3" s="28"/>
+      <c r="AV3" s="31"/>
+      <c r="AW3" s="28"/>
+      <c r="AX3" s="28"/>
+      <c r="AY3" s="29"/>
+      <c r="AZ3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="BA3" s="35"/>
-      <c r="BB3" s="43"/>
-      <c r="BC3" s="35" t="s">
+      <c r="BA3" s="28"/>
+      <c r="BB3" s="36"/>
+      <c r="BC3" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="BD3" s="35"/>
-      <c r="BE3" s="36"/>
-      <c r="BF3" s="34" t="s">
+      <c r="BD3" s="28"/>
+      <c r="BE3" s="31"/>
+      <c r="BF3" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="BG3" s="35"/>
-      <c r="BH3" s="43"/>
-      <c r="BI3" s="35" t="s">
+      <c r="BG3" s="28"/>
+      <c r="BH3" s="36"/>
+      <c r="BI3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="BJ3" s="35"/>
-      <c r="BK3" s="36"/>
-      <c r="BL3" s="35"/>
-      <c r="BM3" s="35"/>
-      <c r="BN3" s="43"/>
-      <c r="BO3" s="35" t="s">
+      <c r="BJ3" s="28"/>
+      <c r="BK3" s="31"/>
+      <c r="BL3" s="28"/>
+      <c r="BM3" s="28"/>
+      <c r="BN3" s="36"/>
+      <c r="BO3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="BP3" s="35"/>
-      <c r="BQ3" s="38"/>
-      <c r="BR3" s="42"/>
-      <c r="BS3" s="42"/>
-      <c r="BT3" s="42"/>
-      <c r="BU3" s="42"/>
-      <c r="BV3" s="42"/>
-      <c r="BW3" s="42"/>
+      <c r="BP3" s="28"/>
+      <c r="BQ3" s="29"/>
+      <c r="BR3" s="37"/>
+      <c r="BS3" s="37"/>
+      <c r="BT3" s="37"/>
+      <c r="BU3" s="37"/>
+      <c r="BV3" s="37"/>
+      <c r="BW3" s="37"/>
     </row>
     <row r="4" spans="1:75" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1755,14 +1956,14 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="36"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="31"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="4" t="s">
@@ -1793,11 +1994,19 @@
         <v>148</v>
       </c>
       <c r="X5" s="6"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="4"/>
+      <c r="Y5" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AA5" s="5"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
+      <c r="AB5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="AD5" s="5"/>
       <c r="AE5" s="4" t="s">
         <v>69</v>
@@ -1812,8 +2021,12 @@
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
       <c r="AM5" s="5"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
+      <c r="AN5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="AP5" s="6"/>
       <c r="AQ5" s="3"/>
       <c r="AR5" s="4"/>
@@ -1832,14 +2045,14 @@
       <c r="BC5" s="4"/>
       <c r="BD5" s="4"/>
       <c r="BE5" s="5"/>
-      <c r="BF5" s="34" t="s">
+      <c r="BF5" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="BG5" s="35"/>
-      <c r="BH5" s="35"/>
-      <c r="BI5" s="35"/>
-      <c r="BJ5" s="35"/>
-      <c r="BK5" s="36"/>
+      <c r="BG5" s="28"/>
+      <c r="BH5" s="28"/>
+      <c r="BI5" s="28"/>
+      <c r="BJ5" s="28"/>
+      <c r="BK5" s="31"/>
       <c r="BL5" s="11"/>
       <c r="BM5" s="11"/>
       <c r="BN5" s="13"/>
@@ -1855,14 +2068,14 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
@@ -1894,11 +2107,19 @@
         <v>148</v>
       </c>
       <c r="X6" s="6"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="4"/>
+      <c r="Y6" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AA6" s="5"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
+      <c r="AB6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>185</v>
+      </c>
       <c r="AD6" s="5"/>
       <c r="AE6" s="4" t="s">
         <v>78</v>
@@ -1913,8 +2134,12 @@
       </c>
       <c r="AL6" s="4"/>
       <c r="AM6" s="5"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
+      <c r="AN6" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="AO6" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="AP6" s="6"/>
       <c r="AQ6" s="3"/>
       <c r="AR6" s="4"/>
@@ -1933,14 +2158,14 @@
       <c r="BC6" s="4"/>
       <c r="BD6" s="4"/>
       <c r="BE6" s="5"/>
-      <c r="BF6" s="34" t="s">
+      <c r="BF6" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="BG6" s="35"/>
-      <c r="BH6" s="35"/>
-      <c r="BI6" s="35"/>
-      <c r="BJ6" s="35"/>
-      <c r="BK6" s="36"/>
+      <c r="BG6" s="28"/>
+      <c r="BH6" s="28"/>
+      <c r="BI6" s="28"/>
+      <c r="BJ6" s="28"/>
+      <c r="BK6" s="31"/>
       <c r="BL6" s="11"/>
       <c r="BM6" s="11"/>
       <c r="BN6" s="13"/>
@@ -1956,14 +2181,14 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="36"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="4" t="s">
         <v>91</v>
       </c>
@@ -1992,14 +2217,26 @@
         <v>144</v>
       </c>
       <c r="U7" s="5"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
+      <c r="V7" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="X7" s="6"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="4"/>
+      <c r="Y7" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z7" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="AA7" s="5"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
+      <c r="AB7" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC7" s="26" t="s">
+        <v>134</v>
+      </c>
       <c r="AD7" s="5"/>
       <c r="AE7" s="4" t="s">
         <v>78</v>
@@ -2047,7 +2284,7 @@
       <c r="BP7" s="11"/>
       <c r="BQ7" s="14"/>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -2055,34 +2292,46 @@
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="38"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="29"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="5"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="5"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
+      <c r="V8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="X8" s="6"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="4"/>
+      <c r="Y8" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z8" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="AA8" s="5"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
+      <c r="AB8" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC8" s="26" t="s">
+        <v>134</v>
+      </c>
       <c r="AD8" s="5"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
@@ -2202,20 +2451,20 @@
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="33"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="40"/>
       <c r="P10" s="9" t="s">
         <v>117</v>
       </c>
@@ -2230,17 +2479,33 @@
         <v>141</v>
       </c>
       <c r="U10" s="12"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
+      <c r="V10" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="W10" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="X10" s="14"/>
-      <c r="Y10" s="9"/>
-      <c r="Z10" s="11"/>
+      <c r="Y10" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z10" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="AA10" s="12"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
+      <c r="AB10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC10" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="AD10" s="12"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
+      <c r="AE10" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF10" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AG10" s="14"/>
       <c r="AH10" s="9"/>
       <c r="AI10" s="11"/>
@@ -2287,20 +2552,20 @@
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="33"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="40"/>
       <c r="P11" s="9" t="s">
         <v>117</v>
       </c>
@@ -2315,17 +2580,33 @@
         <v>141</v>
       </c>
       <c r="U11" s="12"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
+      <c r="V11" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="X11" s="14"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="11"/>
+      <c r="Y11" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z11" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="AA11" s="12"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
+      <c r="AB11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC11" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="AD11" s="12"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
+      <c r="AE11" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF11" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AG11" s="14"/>
       <c r="AH11" s="9"/>
       <c r="AI11" s="11"/>
@@ -2374,14 +2655,14 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="30"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="12"/>
@@ -2406,17 +2687,33 @@
         <v>118</v>
       </c>
       <c r="U12" s="12"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
+      <c r="V12" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="W12" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="X12" s="14"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="11"/>
+      <c r="Y12" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z12" s="11" t="s">
+        <v>177</v>
+      </c>
       <c r="AA12" s="12"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
+      <c r="AB12" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC12" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="AD12" s="12"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
+      <c r="AE12" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF12" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="AG12" s="14"/>
       <c r="AH12" s="9"/>
       <c r="AI12" s="11"/>
@@ -2465,14 +2762,14 @@
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="12"/>
@@ -2493,17 +2790,33 @@
         <v>118</v>
       </c>
       <c r="U13" s="12"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
+      <c r="V13" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="W13" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="X13" s="14"/>
-      <c r="Y13" s="9"/>
-      <c r="Z13" s="11"/>
+      <c r="Y13" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z13" s="11" t="s">
+        <v>177</v>
+      </c>
       <c r="AA13" s="12"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
+      <c r="AB13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC13" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="AD13" s="12"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
+      <c r="AE13" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF13" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AG13" s="14"/>
       <c r="AH13" s="9"/>
       <c r="AI13" s="11"/>
@@ -2564,8 +2877,6 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="14"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="11"/>
       <c r="AA14" s="12"/>
       <c r="AB14" s="11"/>
       <c r="AC14" s="11"/>
@@ -2610,7 +2921,7 @@
       <c r="BP14" s="11"/>
       <c r="BQ14" s="14"/>
     </row>
-    <row r="15" spans="1:75" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2641,8 +2952,12 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="14"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="11"/>
+      <c r="Y15" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z15" s="26" t="s">
+        <v>94</v>
+      </c>
       <c r="AA15" s="12"/>
       <c r="AB15" s="11"/>
       <c r="AC15" s="11"/>
@@ -2696,20 +3011,20 @@
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="33"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="40"/>
       <c r="P16" s="9" t="s">
         <v>58</v>
       </c>
@@ -2724,17 +3039,33 @@
         <v>139</v>
       </c>
       <c r="U16" s="12"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
+      <c r="V16" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="X16" s="14"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="11"/>
+      <c r="Y16" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z16" s="26" t="s">
+        <v>94</v>
+      </c>
       <c r="AA16" s="12"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
+      <c r="AB16" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC16" s="10" t="s">
+        <v>202</v>
+      </c>
       <c r="AD16" s="12"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
+      <c r="AE16" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF16" s="11" t="s">
+        <v>207</v>
+      </c>
       <c r="AG16" s="14"/>
       <c r="AH16" s="9" t="s">
         <v>80</v>
@@ -2782,20 +3113,20 @@
       <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="33"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="40"/>
       <c r="P17" s="9" t="s">
         <v>58</v>
       </c>
@@ -2810,17 +3141,33 @@
         <v>139</v>
       </c>
       <c r="U17" s="12"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
+      <c r="V17" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="W17" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="X17" s="14"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="11"/>
+      <c r="Y17" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z17" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="AA17" s="12"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
+      <c r="AB17" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC17" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="AD17" s="12"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
+      <c r="AE17" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF17" s="11" t="s">
+        <v>207</v>
+      </c>
       <c r="AG17" s="14"/>
       <c r="AH17" s="9"/>
       <c r="AI17" s="11"/>
@@ -3037,7 +3384,6 @@
       <c r="V20" s="11"/>
       <c r="W20" s="11"/>
       <c r="X20" s="14"/>
-      <c r="Z20" s="11"/>
       <c r="AA20" s="12"/>
       <c r="AB20" s="11"/>
       <c r="AC20" s="11"/>
@@ -3091,14 +3437,14 @@
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="30"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="12"/>
@@ -3123,19 +3469,31 @@
         <v>137</v>
       </c>
       <c r="U21" s="12"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
+      <c r="V21" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="W21" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="X21" s="14"/>
       <c r="Y21" s="9" t="s">
         <v>79</v>
       </c>
       <c r="Z21" s="11"/>
       <c r="AA21" s="12"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="11"/>
+      <c r="AB21" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC21" s="11" t="s">
+        <v>187</v>
+      </c>
       <c r="AD21" s="12"/>
-      <c r="AE21" s="11"/>
-      <c r="AF21" s="11"/>
+      <c r="AE21" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF21" s="11" t="s">
+        <v>210</v>
+      </c>
       <c r="AG21" s="14"/>
       <c r="AH21" s="9"/>
       <c r="AI21" s="11"/>
@@ -3155,14 +3513,14 @@
       <c r="AW21" s="11"/>
       <c r="AX21" s="11"/>
       <c r="AY21" s="14"/>
-      <c r="AZ21" s="28" t="s">
+      <c r="AZ21" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="BA21" s="29"/>
-      <c r="BB21" s="29"/>
-      <c r="BC21" s="29"/>
-      <c r="BD21" s="29"/>
-      <c r="BE21" s="30"/>
+      <c r="BA21" s="39"/>
+      <c r="BB21" s="39"/>
+      <c r="BC21" s="39"/>
+      <c r="BD21" s="39"/>
+      <c r="BE21" s="41"/>
       <c r="BF21" s="11"/>
       <c r="BG21" s="11"/>
       <c r="BH21" s="13"/>
@@ -3184,14 +3542,14 @@
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="30"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="12"/>
@@ -3216,19 +3574,31 @@
         <v>137</v>
       </c>
       <c r="U22" s="12"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
+      <c r="V22" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="W22" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="X22" s="14"/>
       <c r="Y22" s="9" t="s">
         <v>79</v>
       </c>
       <c r="Z22" s="11"/>
       <c r="AA22" s="12"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
+      <c r="AB22" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC22" s="11" t="s">
+        <v>187</v>
+      </c>
       <c r="AD22" s="12"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
+      <c r="AE22" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF22" s="11" t="s">
+        <v>210</v>
+      </c>
       <c r="AG22" s="14"/>
       <c r="AH22" s="9"/>
       <c r="AI22" s="11"/>
@@ -3292,8 +3662,12 @@
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
       <c r="U23" s="12"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
+      <c r="V23" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="W23" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="X23" s="14"/>
       <c r="Y23" s="9"/>
       <c r="Z23" s="11"/>
@@ -3419,20 +3793,20 @@
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="33"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="40"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="12"/>
@@ -3496,14 +3870,14 @@
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="30"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="41"/>
       <c r="J26" s="11" t="s">
         <v>92</v>
       </c>
@@ -3518,27 +3892,35 @@
         <v>63</v>
       </c>
       <c r="O26" s="14"/>
-      <c r="P26" s="28" t="s">
+      <c r="P26" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="29"/>
-      <c r="S26" s="29"/>
-      <c r="T26" s="29"/>
-      <c r="U26" s="29"/>
-      <c r="V26" s="29"/>
-      <c r="W26" s="29"/>
-      <c r="X26" s="33"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="11"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="39"/>
+      <c r="T26" s="39"/>
+      <c r="U26" s="39"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="39"/>
+      <c r="X26" s="40"/>
+      <c r="Y26" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z26" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="AA26" s="12"/>
       <c r="AB26" s="15" t="s">
         <v>67</v>
       </c>
       <c r="AC26" s="11"/>
       <c r="AD26" s="11"/>
-      <c r="AE26" s="11"/>
-      <c r="AF26" s="11"/>
+      <c r="AE26" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF26" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="AG26" s="14"/>
       <c r="AH26" s="9"/>
       <c r="AI26" s="11"/>
@@ -3587,14 +3969,14 @@
       <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="30"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="41"/>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
       <c r="L27" s="12"/>
@@ -3605,25 +3987,37 @@
         <v>63</v>
       </c>
       <c r="O27" s="14"/>
-      <c r="P27" s="28" t="s">
+      <c r="P27" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="29"/>
-      <c r="T27" s="29"/>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="29"/>
-      <c r="X27" s="33"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="11"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
+      <c r="T27" s="39"/>
+      <c r="U27" s="39"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="40"/>
+      <c r="Y27" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z27" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="AA27" s="12"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
+      <c r="AB27" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC27" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="AD27" s="12"/>
-      <c r="AE27" s="11"/>
-      <c r="AF27" s="11"/>
+      <c r="AE27" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="AG27" s="14"/>
       <c r="AH27" s="9"/>
       <c r="AI27" s="11"/>
@@ -3662,7 +4056,7 @@
       <c r="BP27" s="11"/>
       <c r="BQ27" s="14"/>
     </row>
-    <row r="28" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:69" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>3</v>
@@ -3694,8 +4088,12 @@
       <c r="Y28" s="9"/>
       <c r="Z28" s="11"/>
       <c r="AA28" s="12"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
+      <c r="AB28" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC28" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="AD28" s="12"/>
       <c r="AE28" s="11"/>
       <c r="AF28" s="11"/>
@@ -3737,7 +4135,7 @@
       <c r="BP28" s="11"/>
       <c r="BQ28" s="14"/>
     </row>
-    <row r="29" spans="1:69" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:69" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="9"/>
       <c r="E29" s="11"/>
       <c r="F29" s="12"/>
@@ -3898,20 +4296,20 @@
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="33"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="40"/>
       <c r="P31" s="9" t="s">
         <v>120</v>
       </c>
@@ -3926,29 +4324,45 @@
         <v>139</v>
       </c>
       <c r="U31" s="12"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
+      <c r="V31" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="W31" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="X31" s="14"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="11"/>
+      <c r="Y31" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z31" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="AA31" s="12"/>
-      <c r="AB31" s="11"/>
-      <c r="AC31" s="11"/>
+      <c r="AB31" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC31" s="11" t="s">
+        <v>185</v>
+      </c>
       <c r="AD31" s="12"/>
-      <c r="AE31" s="11"/>
-      <c r="AF31" s="11"/>
+      <c r="AE31" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF31" s="11" t="s">
+        <v>210</v>
+      </c>
       <c r="AG31" s="14"/>
       <c r="AH31" s="9"/>
       <c r="AI31" s="11"/>
       <c r="AJ31" s="12"/>
-      <c r="AK31" s="32" t="s">
+      <c r="AK31" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="AL31" s="29"/>
-      <c r="AM31" s="29"/>
-      <c r="AN31" s="29"/>
-      <c r="AO31" s="29"/>
-      <c r="AP31" s="33"/>
+      <c r="AL31" s="39"/>
+      <c r="AM31" s="39"/>
+      <c r="AN31" s="39"/>
+      <c r="AO31" s="39"/>
+      <c r="AP31" s="40"/>
       <c r="AQ31" s="9"/>
       <c r="AR31" s="11"/>
       <c r="AS31" s="12"/>
@@ -3983,20 +4397,20 @@
       <c r="C32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="33"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="40"/>
       <c r="P32" s="9" t="s">
         <v>58</v>
       </c>
@@ -4010,26 +4424,38 @@
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
       <c r="X32" s="14"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="11"/>
+      <c r="Y32" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z32" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="AA32" s="12"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
+      <c r="AB32" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC32" s="11" t="s">
+        <v>185</v>
+      </c>
       <c r="AD32" s="12"/>
-      <c r="AE32" s="11"/>
-      <c r="AF32" s="11"/>
+      <c r="AE32" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF32" s="11" t="s">
+        <v>210</v>
+      </c>
       <c r="AG32" s="14"/>
       <c r="AH32" s="9"/>
       <c r="AI32" s="11"/>
       <c r="AJ32" s="12"/>
-      <c r="AK32" s="32" t="s">
+      <c r="AK32" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="AL32" s="29"/>
-      <c r="AM32" s="29"/>
-      <c r="AN32" s="29"/>
-      <c r="AO32" s="29"/>
-      <c r="AP32" s="33"/>
+      <c r="AL32" s="39"/>
+      <c r="AM32" s="39"/>
+      <c r="AN32" s="39"/>
+      <c r="AO32" s="39"/>
+      <c r="AP32" s="40"/>
       <c r="AQ32" s="9"/>
       <c r="AR32" s="11"/>
       <c r="AS32" s="12"/>
@@ -4135,14 +4561,14 @@
       <c r="C34" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="30"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="41"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
       <c r="L34" s="12"/>
@@ -4281,7 +4707,7 @@
       <c r="BP35" s="11"/>
       <c r="BQ35" s="14"/>
     </row>
-    <row r="36" spans="1:69" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:69" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
         <v>1</v>
@@ -4289,14 +4715,14 @@
       <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="30"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="41"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="12"/>
@@ -4307,27 +4733,35 @@
         <v>63</v>
       </c>
       <c r="O36" s="14"/>
-      <c r="P36" s="28" t="s">
+      <c r="P36" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="29"/>
-      <c r="X36" s="33"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39"/>
+      <c r="S36" s="39"/>
+      <c r="T36" s="39"/>
+      <c r="U36" s="39"/>
+      <c r="V36" s="39"/>
+      <c r="W36" s="39"/>
+      <c r="X36" s="40"/>
       <c r="Y36" s="9" t="s">
         <v>79</v>
       </c>
       <c r="Z36" s="11"/>
       <c r="AA36" s="12"/>
-      <c r="AB36" s="11"/>
-      <c r="AC36" s="11"/>
+      <c r="AB36" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC36" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="AD36" s="12"/>
-      <c r="AE36" s="11"/>
-      <c r="AF36" s="11"/>
+      <c r="AE36" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF36" s="11" t="s">
+        <v>210</v>
+      </c>
       <c r="AG36" s="14"/>
       <c r="AH36" s="9"/>
       <c r="AI36" s="11"/>
@@ -4374,14 +4808,14 @@
       <c r="C37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="30"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="41"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="12"/>
@@ -4396,17 +4830,33 @@
       <c r="S37" s="11"/>
       <c r="T37" s="11"/>
       <c r="U37" s="12"/>
-      <c r="V37" s="11"/>
-      <c r="W37" s="11"/>
+      <c r="V37" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="W37" s="11" t="s">
+        <v>164</v>
+      </c>
       <c r="X37" s="14"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="11"/>
+      <c r="Y37" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z37" s="10" t="s">
+        <v>173</v>
+      </c>
       <c r="AA37" s="12"/>
-      <c r="AB37" s="11"/>
-      <c r="AC37" s="11"/>
+      <c r="AB37" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC37" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="AD37" s="12"/>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="11"/>
+      <c r="AE37" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF37" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG37" s="14"/>
       <c r="AH37" s="9"/>
       <c r="AI37" s="11"/>
@@ -4478,14 +4928,22 @@
       <c r="V38" s="11"/>
       <c r="W38" s="11"/>
       <c r="X38" s="14"/>
-      <c r="Y38" s="9"/>
-      <c r="Z38" s="11"/>
+      <c r="Y38" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z38" s="10" t="s">
+        <v>173</v>
+      </c>
       <c r="AA38" s="12"/>
       <c r="AB38" s="11"/>
       <c r="AC38" s="11"/>
       <c r="AD38" s="12"/>
-      <c r="AE38" s="11"/>
-      <c r="AF38" s="11"/>
+      <c r="AE38" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF38" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG38" s="14"/>
       <c r="AH38" s="9"/>
       <c r="AI38" s="11"/>
@@ -4602,20 +5060,20 @@
       <c r="C40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="37" t="s">
+      <c r="D40" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="38"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="29"/>
       <c r="P40" s="9" t="s">
         <v>128</v>
       </c>
@@ -4635,14 +5093,26 @@
       </c>
       <c r="W40" s="11"/>
       <c r="X40" s="14"/>
-      <c r="Y40" s="9"/>
-      <c r="Z40" s="11"/>
+      <c r="Y40" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z40" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="AA40" s="12"/>
-      <c r="AB40" s="11"/>
-      <c r="AC40" s="11"/>
+      <c r="AB40" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC40" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AD40" s="12"/>
-      <c r="AE40" s="11"/>
-      <c r="AF40" s="11"/>
+      <c r="AE40" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF40" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="AG40" s="14"/>
       <c r="AH40" s="9"/>
       <c r="AI40" s="11"/>
@@ -4668,14 +5138,14 @@
       <c r="BC40" s="11"/>
       <c r="BD40" s="11"/>
       <c r="BE40" s="12"/>
-      <c r="BF40" s="34" t="s">
+      <c r="BF40" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="BG40" s="35"/>
-      <c r="BH40" s="35"/>
-      <c r="BI40" s="35"/>
-      <c r="BJ40" s="35"/>
-      <c r="BK40" s="36"/>
+      <c r="BG40" s="28"/>
+      <c r="BH40" s="28"/>
+      <c r="BI40" s="28"/>
+      <c r="BJ40" s="28"/>
+      <c r="BK40" s="31"/>
       <c r="BL40" s="11"/>
       <c r="BM40" s="11"/>
       <c r="BN40" s="13"/>
@@ -4691,20 +5161,20 @@
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="38"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="29"/>
       <c r="P41" s="9" t="s">
         <v>128</v>
       </c>
@@ -4724,14 +5194,26 @@
       </c>
       <c r="W41" s="11"/>
       <c r="X41" s="14"/>
-      <c r="Y41" s="9"/>
-      <c r="Z41" s="11"/>
+      <c r="Y41" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z41" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="AA41" s="12"/>
-      <c r="AB41" s="11"/>
-      <c r="AC41" s="11"/>
+      <c r="AB41" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC41" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AD41" s="12"/>
-      <c r="AE41" s="11"/>
-      <c r="AF41" s="11"/>
+      <c r="AE41" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF41" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="AG41" s="14"/>
       <c r="AH41" s="9"/>
       <c r="AI41" s="11"/>
@@ -4778,14 +5260,14 @@
       <c r="C42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D42" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="30"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="41"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
       <c r="L42" s="12"/>
@@ -4806,17 +5288,33 @@
       <c r="S42" s="11"/>
       <c r="T42" s="11"/>
       <c r="U42" s="12"/>
-      <c r="V42" s="11"/>
-      <c r="W42" s="11"/>
+      <c r="V42" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="W42" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="X42" s="14"/>
-      <c r="Y42" s="9"/>
-      <c r="Z42" s="11"/>
+      <c r="Y42" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z42" s="11" t="s">
+        <v>183</v>
+      </c>
       <c r="AA42" s="12"/>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="11"/>
+      <c r="AB42" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC42" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="AD42" s="12"/>
-      <c r="AE42" s="11"/>
-      <c r="AF42" s="11"/>
+      <c r="AE42" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF42" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AG42" s="14"/>
       <c r="AH42" s="9"/>
       <c r="AI42" s="11"/>
@@ -4865,14 +5363,14 @@
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="30"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="41"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
       <c r="L43" s="12"/>
@@ -4893,17 +5391,33 @@
       <c r="S43" s="11"/>
       <c r="T43" s="11"/>
       <c r="U43" s="12"/>
-      <c r="V43" s="11"/>
-      <c r="W43" s="11"/>
+      <c r="V43" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="W43" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="X43" s="14"/>
-      <c r="Y43" s="9"/>
-      <c r="Z43" s="11"/>
+      <c r="Y43" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z43" s="11" t="s">
+        <v>183</v>
+      </c>
       <c r="AA43" s="12"/>
-      <c r="AB43" s="11"/>
-      <c r="AC43" s="11"/>
+      <c r="AB43" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC43" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="AD43" s="12"/>
-      <c r="AE43" s="11"/>
-      <c r="AF43" s="11"/>
+      <c r="AE43" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF43" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AG43" s="14"/>
       <c r="AH43" s="9"/>
       <c r="AI43" s="11"/>
@@ -5022,14 +5536,14 @@
       <c r="C45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="31"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="45"/>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
       <c r="L45" s="12"/>
@@ -5050,15 +5564,33 @@
       <c r="S45" s="11"/>
       <c r="T45" s="11"/>
       <c r="U45" s="12"/>
+      <c r="V45" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="W45" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="X45" s="14"/>
-      <c r="Y45" s="9"/>
-      <c r="Z45" s="11"/>
+      <c r="Y45" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z45" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="AA45" s="12"/>
-      <c r="AB45" s="11"/>
-      <c r="AC45" s="11"/>
+      <c r="AB45" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC45" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="AD45" s="12"/>
-      <c r="AE45" s="11"/>
-      <c r="AF45" s="11"/>
+      <c r="AE45" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF45" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG45" s="14"/>
       <c r="AH45" s="9"/>
       <c r="AI45" s="11"/>
@@ -5105,14 +5637,14 @@
       <c r="C46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="31"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="45"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
       <c r="L46" s="12"/>
@@ -5133,15 +5665,33 @@
       <c r="S46" s="11"/>
       <c r="T46" s="11"/>
       <c r="U46" s="12"/>
+      <c r="V46" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="W46" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="X46" s="14"/>
-      <c r="Y46" s="9"/>
-      <c r="Z46" s="11"/>
+      <c r="Y46" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z46" s="11" t="s">
+        <v>177</v>
+      </c>
       <c r="AA46" s="12"/>
-      <c r="AB46" s="11"/>
-      <c r="AC46" s="11"/>
+      <c r="AB46" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC46" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="AD46" s="12"/>
-      <c r="AE46" s="11"/>
-      <c r="AF46" s="11"/>
+      <c r="AE46" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF46" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG46" s="14"/>
       <c r="AH46" s="9"/>
       <c r="AI46" s="11"/>
@@ -5184,7 +5734,7 @@
       <c r="BP46" s="11"/>
       <c r="BQ46" s="14"/>
     </row>
-    <row r="47" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:69" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
         <v>2</v>
@@ -5204,25 +5754,37 @@
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
       <c r="O47" s="14"/>
-      <c r="P47" s="28" t="s">
+      <c r="P47" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="Q47" s="29"/>
-      <c r="R47" s="29"/>
-      <c r="S47" s="29"/>
-      <c r="T47" s="29"/>
-      <c r="U47" s="29"/>
-      <c r="V47" s="29"/>
-      <c r="W47" s="29"/>
-      <c r="X47" s="33"/>
-      <c r="Y47" s="9"/>
-      <c r="Z47" s="11"/>
+      <c r="Q47" s="39"/>
+      <c r="R47" s="39"/>
+      <c r="S47" s="39"/>
+      <c r="T47" s="39"/>
+      <c r="U47" s="39"/>
+      <c r="V47" s="39"/>
+      <c r="W47" s="39"/>
+      <c r="X47" s="40"/>
+      <c r="Y47" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z47" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="AA47" s="12"/>
-      <c r="AB47" s="11"/>
-      <c r="AC47" s="11"/>
+      <c r="AB47" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC47" s="11" t="s">
+        <v>195</v>
+      </c>
       <c r="AD47" s="12"/>
-      <c r="AE47" s="11"/>
-      <c r="AF47" s="11"/>
+      <c r="AE47" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF47" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="AG47" s="14"/>
       <c r="AH47" s="9"/>
       <c r="AI47" s="11"/>
@@ -5261,7 +5823,7 @@
       <c r="BP47" s="11"/>
       <c r="BQ47" s="14"/>
     </row>
-    <row r="48" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:69" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
         <v>3</v>
@@ -5281,19 +5843,23 @@
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
       <c r="O48" s="14"/>
-      <c r="P48" s="28" t="s">
+      <c r="P48" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="Q48" s="29"/>
-      <c r="R48" s="29"/>
-      <c r="S48" s="29"/>
-      <c r="T48" s="29"/>
-      <c r="U48" s="29"/>
-      <c r="V48" s="29"/>
-      <c r="W48" s="29"/>
-      <c r="X48" s="33"/>
-      <c r="Y48" s="11"/>
-      <c r="Z48" s="11"/>
+      <c r="Q48" s="39"/>
+      <c r="R48" s="39"/>
+      <c r="S48" s="39"/>
+      <c r="T48" s="39"/>
+      <c r="U48" s="39"/>
+      <c r="V48" s="39"/>
+      <c r="W48" s="39"/>
+      <c r="X48" s="40"/>
+      <c r="Y48" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z48" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="AA48" s="11"/>
       <c r="AB48" s="11"/>
       <c r="AC48" s="11"/>
@@ -5413,7 +5979,7 @@
       <c r="BP49" s="11"/>
       <c r="BQ49" s="14"/>
     </row>
-    <row r="50" spans="1:69" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:69" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
@@ -5444,8 +6010,12 @@
       <c r="V50" s="11"/>
       <c r="W50" s="11"/>
       <c r="X50" s="14"/>
-      <c r="Y50" s="11"/>
-      <c r="Z50" s="11"/>
+      <c r="Y50" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z50" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="AA50" s="11"/>
       <c r="AB50" s="15"/>
       <c r="AC50" s="11"/>
@@ -5471,14 +6041,14 @@
       <c r="AW50" s="11"/>
       <c r="AX50" s="11"/>
       <c r="AY50" s="14"/>
-      <c r="AZ50" s="28" t="s">
+      <c r="AZ50" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="BA50" s="29"/>
-      <c r="BB50" s="29"/>
-      <c r="BC50" s="29"/>
-      <c r="BD50" s="29"/>
-      <c r="BE50" s="30"/>
+      <c r="BA50" s="39"/>
+      <c r="BB50" s="39"/>
+      <c r="BC50" s="39"/>
+      <c r="BD50" s="39"/>
+      <c r="BE50" s="41"/>
       <c r="BF50" s="11"/>
       <c r="BG50" s="11"/>
       <c r="BH50" s="13"/>
@@ -5503,14 +6073,14 @@
       <c r="D51" s="9"/>
       <c r="E51" s="11"/>
       <c r="F51" s="12"/>
-      <c r="G51" s="32" t="s">
+      <c r="G51" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="30"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="39"/>
+      <c r="L51" s="41"/>
       <c r="M51" s="10" t="s">
         <v>89</v>
       </c>
@@ -5532,14 +6102,26 @@
         <v>107</v>
       </c>
       <c r="U51" s="12"/>
-      <c r="V51" s="11"/>
-      <c r="W51" s="11"/>
+      <c r="V51" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="W51" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="X51" s="14"/>
-      <c r="Y51" s="11"/>
-      <c r="Z51" s="11"/>
+      <c r="Y51" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z51" s="11" t="s">
+        <v>172</v>
+      </c>
       <c r="AA51" s="11"/>
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="11"/>
+      <c r="AB51" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC51" s="11" t="s">
+        <v>189</v>
+      </c>
       <c r="AD51" s="12"/>
       <c r="AE51" s="4" t="s">
         <v>71</v>
@@ -5551,14 +6133,14 @@
       <c r="AH51" s="11"/>
       <c r="AI51" s="11"/>
       <c r="AJ51" s="12"/>
-      <c r="AK51" s="32" t="s">
+      <c r="AK51" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="AL51" s="29"/>
-      <c r="AM51" s="29"/>
-      <c r="AN51" s="29"/>
-      <c r="AO51" s="29"/>
-      <c r="AP51" s="33"/>
+      <c r="AL51" s="39"/>
+      <c r="AM51" s="39"/>
+      <c r="AN51" s="39"/>
+      <c r="AO51" s="39"/>
+      <c r="AP51" s="40"/>
       <c r="AQ51" s="11"/>
       <c r="AR51" s="11"/>
       <c r="AS51" s="12"/>
@@ -5592,14 +6174,14 @@
       <c r="D52" s="9"/>
       <c r="E52" s="11"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="32" t="s">
+      <c r="G52" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="30"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="41"/>
       <c r="M52" s="10" t="s">
         <v>89</v>
       </c>
@@ -5621,14 +6203,26 @@
         <v>107</v>
       </c>
       <c r="U52" s="12"/>
-      <c r="V52" s="11"/>
-      <c r="W52" s="11"/>
+      <c r="V52" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="W52" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="X52" s="14"/>
-      <c r="Y52" s="11"/>
-      <c r="Z52" s="11"/>
+      <c r="Y52" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z52" s="11" t="s">
+        <v>172</v>
+      </c>
       <c r="AA52" s="11"/>
-      <c r="AB52" s="15"/>
-      <c r="AC52" s="11"/>
+      <c r="AB52" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC52" s="11" t="s">
+        <v>189</v>
+      </c>
       <c r="AD52" s="12"/>
       <c r="AE52" s="11"/>
       <c r="AF52" s="11"/>
@@ -5755,14 +6349,14 @@
       <c r="D54" s="9"/>
       <c r="E54" s="11"/>
       <c r="F54" s="12"/>
-      <c r="G54" s="32" t="s">
+      <c r="G54" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="30"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="41"/>
       <c r="M54" s="11"/>
       <c r="N54" s="11"/>
       <c r="O54" s="14"/>
@@ -5834,14 +6428,14 @@
       <c r="D55" s="9"/>
       <c r="E55" s="11"/>
       <c r="F55" s="12"/>
-      <c r="G55" s="32" t="s">
+      <c r="G55" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="30"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="39"/>
+      <c r="L55" s="41"/>
       <c r="M55" s="11"/>
       <c r="N55" s="11"/>
       <c r="O55" s="14"/>
@@ -5908,14 +6502,14 @@
       <c r="C56" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="26" t="s">
+      <c r="D56" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
       <c r="M56" s="11" t="s">
         <v>109</v>
       </c>
@@ -5940,14 +6534,26 @@
       <c r="V56" s="11"/>
       <c r="W56" s="11"/>
       <c r="X56" s="14"/>
-      <c r="Y56" s="11"/>
-      <c r="Z56" s="11"/>
+      <c r="Y56" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z56" s="10" t="s">
+        <v>173</v>
+      </c>
       <c r="AA56" s="11"/>
-      <c r="AB56" s="15"/>
-      <c r="AC56" s="11"/>
+      <c r="AB56" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC56" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="AD56" s="12"/>
-      <c r="AE56" s="11"/>
-      <c r="AF56" s="11"/>
+      <c r="AE56" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF56" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG56" s="14"/>
       <c r="AH56" s="11"/>
       <c r="AI56" s="11"/>
@@ -5994,14 +6600,14 @@
       <c r="C57" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D57" s="26" t="s">
+      <c r="D57" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
       <c r="M57" s="11" t="s">
         <v>109</v>
       </c>
@@ -6018,17 +6624,33 @@
       <c r="R57" s="12"/>
       <c r="T57" s="11"/>
       <c r="U57" s="12"/>
-      <c r="V57" s="11"/>
-      <c r="W57" s="11"/>
+      <c r="V57" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="W57" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="X57" s="14"/>
-      <c r="Y57" s="11"/>
-      <c r="Z57" s="11"/>
+      <c r="Y57" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z57" s="11" t="s">
+        <v>172</v>
+      </c>
       <c r="AA57" s="11"/>
-      <c r="AB57" s="15"/>
-      <c r="AC57" s="11"/>
+      <c r="AB57" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC57" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="AD57" s="12"/>
-      <c r="AE57" s="11"/>
-      <c r="AF57" s="11"/>
+      <c r="AE57" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF57" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG57" s="14"/>
       <c r="AH57" s="11"/>
       <c r="AI57" s="11"/>
@@ -6067,7 +6689,7 @@
       <c r="BP57" s="11"/>
       <c r="BQ57" s="14"/>
     </row>
-    <row r="58" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:69" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
         <v>3</v>
@@ -6093,8 +6715,12 @@
       <c r="S58" s="11"/>
       <c r="T58" s="11"/>
       <c r="U58" s="12"/>
-      <c r="V58" s="11"/>
-      <c r="W58" s="11"/>
+      <c r="V58" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="W58" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="X58" s="14"/>
       <c r="Y58" s="11"/>
       <c r="Z58" s="11"/>
@@ -6234,14 +6860,14 @@
       <c r="D60" s="9"/>
       <c r="E60" s="11"/>
       <c r="F60" s="12"/>
-      <c r="G60" s="32" t="s">
+      <c r="G60" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H60" s="29"/>
-      <c r="I60" s="29"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="30"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="41"/>
       <c r="M60" s="11"/>
       <c r="N60" s="11"/>
       <c r="O60" s="14"/>
@@ -6308,14 +6934,14 @@
       <c r="C61" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G61" s="32" t="s">
+      <c r="G61" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="H61" s="29"/>
-      <c r="I61" s="29"/>
-      <c r="J61" s="29"/>
-      <c r="K61" s="29"/>
-      <c r="L61" s="30"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="39"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="39"/>
+      <c r="L61" s="41"/>
       <c r="M61" s="11"/>
       <c r="N61" s="11"/>
       <c r="O61" s="14"/>
@@ -6336,8 +6962,12 @@
         <v>150</v>
       </c>
       <c r="X61" s="14"/>
-      <c r="Y61" s="11"/>
-      <c r="Z61" s="11"/>
+      <c r="Y61" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z61" s="10" t="s">
+        <v>173</v>
+      </c>
       <c r="AA61" s="11"/>
       <c r="AB61" s="15" t="s">
         <v>68</v>
@@ -6394,14 +7024,14 @@
       <c r="C62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
-      <c r="I62" s="30"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="41"/>
       <c r="K62" s="11"/>
       <c r="L62" s="12"/>
       <c r="M62" s="11"/>
@@ -6424,14 +7054,26 @@
         <v>150</v>
       </c>
       <c r="X62" s="14"/>
-      <c r="Y62" s="11"/>
-      <c r="Z62" s="11"/>
+      <c r="Y62" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z62" s="11" t="s">
+        <v>172</v>
+      </c>
       <c r="AA62" s="11"/>
-      <c r="AB62" s="15"/>
-      <c r="AC62" s="11"/>
+      <c r="AB62" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC62" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="AD62" s="12"/>
-      <c r="AE62" s="11"/>
-      <c r="AF62" s="11"/>
+      <c r="AE62" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF62" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="AG62" s="14"/>
       <c r="AH62" s="11"/>
       <c r="AI62" s="11"/>
@@ -6470,7 +7112,7 @@
       <c r="BP62" s="11"/>
       <c r="BQ62" s="14"/>
     </row>
-    <row r="63" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:69" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
         <v>3</v>
@@ -6499,14 +7141,22 @@
       <c r="V63" s="11"/>
       <c r="W63" s="11"/>
       <c r="X63" s="14"/>
-      <c r="Y63" s="11"/>
-      <c r="Z63" s="11"/>
+      <c r="Y63" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z63" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="AA63" s="11"/>
       <c r="AB63" s="15"/>
       <c r="AC63" s="11"/>
       <c r="AD63" s="12"/>
-      <c r="AE63" s="11"/>
-      <c r="AF63" s="11"/>
+      <c r="AE63" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF63" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="AG63" s="14"/>
       <c r="AH63" s="11"/>
       <c r="AI63" s="11"/>
@@ -6662,11 +7312,19 @@
       <c r="Y65" s="11"/>
       <c r="Z65" s="11"/>
       <c r="AA65" s="11"/>
-      <c r="AB65" s="15"/>
-      <c r="AC65" s="11"/>
+      <c r="AB65" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC65" s="11" t="s">
+        <v>187</v>
+      </c>
       <c r="AD65" s="12"/>
-      <c r="AE65" s="11"/>
-      <c r="AF65" s="11"/>
+      <c r="AE65" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF65" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG65" s="14"/>
       <c r="AH65" s="11"/>
       <c r="AI65" s="11"/>
@@ -6720,12 +7378,12 @@
         <v>111</v>
       </c>
       <c r="F66" s="12"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="29"/>
-      <c r="I66" s="29"/>
-      <c r="J66" s="29"/>
-      <c r="K66" s="29"/>
-      <c r="L66" s="30"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="39"/>
+      <c r="J66" s="39"/>
+      <c r="K66" s="39"/>
+      <c r="L66" s="41"/>
       <c r="M66" s="11" t="s">
         <v>108</v>
       </c>
@@ -6747,17 +7405,33 @@
         <v>141</v>
       </c>
       <c r="U66" s="12"/>
-      <c r="V66" s="11"/>
-      <c r="W66" s="11"/>
+      <c r="V66" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="W66" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="X66" s="14"/>
-      <c r="Y66" s="11"/>
-      <c r="Z66" s="11"/>
+      <c r="Y66" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z66" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="AA66" s="11"/>
-      <c r="AB66" s="15"/>
-      <c r="AC66" s="11"/>
+      <c r="AB66" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC66" s="11" t="s">
+        <v>192</v>
+      </c>
       <c r="AD66" s="12"/>
-      <c r="AE66" s="11"/>
-      <c r="AF66" s="11"/>
+      <c r="AE66" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF66" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG66" s="14"/>
       <c r="AH66" s="11"/>
       <c r="AI66" s="11"/>
@@ -6811,12 +7485,12 @@
         <v>111</v>
       </c>
       <c r="F67" s="12"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="29"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="30"/>
+      <c r="G67" s="42"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="39"/>
+      <c r="J67" s="39"/>
+      <c r="K67" s="39"/>
+      <c r="L67" s="41"/>
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
       <c r="O67" s="14"/>
@@ -6828,11 +7502,13 @@
       </c>
       <c r="R67" s="12"/>
       <c r="U67" s="12"/>
-      <c r="V67" s="11"/>
-      <c r="W67" s="11"/>
+      <c r="V67" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="W67" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="X67" s="14"/>
-      <c r="Y67" s="11"/>
-      <c r="Z67" s="11"/>
       <c r="AA67" s="11"/>
       <c r="AB67" s="15"/>
       <c r="AC67" s="11"/>
@@ -7055,8 +7731,12 @@
       <c r="AB70" s="15"/>
       <c r="AC70" s="11"/>
       <c r="AD70" s="12"/>
-      <c r="AE70" s="11"/>
-      <c r="AF70" s="11"/>
+      <c r="AE70" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF70" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="AG70" s="14"/>
       <c r="AH70" s="11"/>
       <c r="AI70" s="11"/>
@@ -7103,14 +7783,14 @@
       <c r="C71" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D71" s="28" t="s">
+      <c r="D71" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="29"/>
-      <c r="I71" s="30"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="41"/>
       <c r="J71" s="11"/>
       <c r="K71" s="11"/>
       <c r="L71" s="12"/>
@@ -7131,17 +7811,29 @@
         <v>134</v>
       </c>
       <c r="U71" s="12"/>
-      <c r="V71" s="11"/>
-      <c r="W71" s="11"/>
+      <c r="V71" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="W71" s="10" t="s">
+        <v>110</v>
+      </c>
       <c r="X71" s="14"/>
-      <c r="Y71" s="11"/>
-      <c r="Z71" s="11"/>
+      <c r="Y71" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z71" s="10" t="s">
+        <v>183</v>
+      </c>
       <c r="AA71" s="11"/>
       <c r="AB71" s="15"/>
       <c r="AC71" s="11"/>
       <c r="AD71" s="12"/>
-      <c r="AE71" s="11"/>
-      <c r="AF71" s="11"/>
+      <c r="AE71" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF71" s="10" t="s">
+        <v>214</v>
+      </c>
       <c r="AG71" s="14"/>
       <c r="AH71" s="11"/>
       <c r="AI71" s="11"/>
@@ -7188,14 +7880,14 @@
       <c r="C72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D72" s="26" t="s">
+      <c r="D72" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="31"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="45"/>
       <c r="J72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="12"/>
@@ -7216,17 +7908,33 @@
         <v>141</v>
       </c>
       <c r="U72" s="12"/>
-      <c r="V72" s="11"/>
-      <c r="W72" s="11"/>
+      <c r="V72" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="W72" s="11" t="s">
+        <v>159</v>
+      </c>
       <c r="X72" s="14"/>
-      <c r="Y72" s="11"/>
-      <c r="Z72" s="11"/>
+      <c r="Y72" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z72" s="11" t="s">
+        <v>172</v>
+      </c>
       <c r="AA72" s="11"/>
-      <c r="AB72" s="15"/>
-      <c r="AC72" s="11"/>
+      <c r="AB72" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC72" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="AD72" s="12"/>
-      <c r="AE72" s="11"/>
-      <c r="AF72" s="11"/>
+      <c r="AE72" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="AF72" s="11" t="s">
+        <v>214</v>
+      </c>
       <c r="AG72" s="14"/>
       <c r="AH72" s="11"/>
       <c r="AI72" s="11"/>
@@ -7273,14 +7981,14 @@
       <c r="C73" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D73" s="26" t="s">
+      <c r="D73" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
-      <c r="I73" s="31"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="45"/>
       <c r="J73" s="11"/>
       <c r="K73" s="11"/>
       <c r="L73" s="12"/>
@@ -7424,14 +8132,14 @@
       <c r="C75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="26" t="s">
+      <c r="D75" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="31"/>
+      <c r="E75" s="44"/>
+      <c r="F75" s="44"/>
+      <c r="G75" s="44"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="45"/>
       <c r="J75" s="11"/>
       <c r="K75" s="11"/>
       <c r="L75" s="12"/>
@@ -7450,8 +8158,12 @@
       <c r="Y75" s="11"/>
       <c r="Z75" s="11"/>
       <c r="AA75" s="11"/>
-      <c r="AB75" s="15"/>
-      <c r="AC75" s="11"/>
+      <c r="AB75" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC75" s="11" t="s">
+        <v>141</v>
+      </c>
       <c r="AD75" s="12"/>
       <c r="AE75" s="11"/>
       <c r="AF75" s="11"/>
@@ -7501,14 +8213,14 @@
       <c r="C76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="26" t="s">
+      <c r="D76" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="44"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="44"/>
       <c r="J76" s="11"/>
       <c r="K76" s="11"/>
       <c r="L76" s="12"/>
@@ -7526,11 +8238,19 @@
         <v>150</v>
       </c>
       <c r="X76" s="14"/>
-      <c r="Y76" s="11"/>
-      <c r="Z76" s="11"/>
+      <c r="Y76" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z76" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="AA76" s="11"/>
-      <c r="AB76" s="15"/>
-      <c r="AC76" s="11"/>
+      <c r="AB76" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC76" s="11" t="s">
+        <v>141</v>
+      </c>
       <c r="AD76" s="12"/>
       <c r="AE76" s="11"/>
       <c r="AF76" s="11"/>
@@ -7580,14 +8300,14 @@
       <c r="C77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D77" s="26" t="s">
+      <c r="D77" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="44"/>
+      <c r="I77" s="44"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11"/>
       <c r="L77" s="12"/>
@@ -7604,14 +8324,26 @@
       <c r="S77" s="11"/>
       <c r="T77" s="11"/>
       <c r="U77" s="12"/>
-      <c r="V77" s="11"/>
-      <c r="W77" s="11"/>
+      <c r="V77" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="W77" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="X77" s="14"/>
-      <c r="Y77" s="11"/>
-      <c r="Z77" s="11"/>
+      <c r="Y77" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z77" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="AA77" s="11"/>
-      <c r="AB77" s="15"/>
-      <c r="AC77" s="11"/>
+      <c r="AB77" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC77" s="11" t="s">
+        <v>199</v>
+      </c>
       <c r="AD77" s="12"/>
       <c r="AE77" s="11"/>
       <c r="AF77" s="11"/>
@@ -7661,14 +8393,14 @@
       <c r="C78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="28" t="s">
+      <c r="D78" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="29"/>
-      <c r="I78" s="30"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="39"/>
+      <c r="H78" s="39"/>
+      <c r="I78" s="41"/>
       <c r="J78" s="11"/>
       <c r="K78" s="11"/>
       <c r="L78" s="12"/>
@@ -7685,11 +8417,19 @@
       <c r="S78" s="11"/>
       <c r="T78" s="11"/>
       <c r="U78" s="12"/>
-      <c r="V78" s="11"/>
-      <c r="W78" s="11"/>
+      <c r="V78" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="W78" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="X78" s="14"/>
-      <c r="Y78" s="11"/>
-      <c r="Z78" s="11"/>
+      <c r="Y78" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z78" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="AA78" s="11"/>
       <c r="AB78" s="15"/>
       <c r="AC78" s="11"/>
@@ -7806,14 +8546,14 @@
       <c r="C80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="26" t="s">
+      <c r="D80" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="44"/>
       <c r="J80" s="11"/>
       <c r="K80" s="11"/>
       <c r="L80" s="12"/>
@@ -7883,14 +8623,14 @@
       <c r="C81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="28" t="s">
+      <c r="D81" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
-      <c r="G81" s="29"/>
-      <c r="H81" s="29"/>
-      <c r="I81" s="30"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="39"/>
+      <c r="H81" s="39"/>
+      <c r="I81" s="41"/>
       <c r="J81" s="11"/>
       <c r="K81" s="11"/>
       <c r="L81" s="12"/>
@@ -7906,8 +8646,12 @@
       <c r="V81" s="11"/>
       <c r="W81" s="11"/>
       <c r="X81" s="14"/>
-      <c r="Y81" s="11"/>
-      <c r="Z81" s="11"/>
+      <c r="Y81" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z81" s="11" t="s">
+        <v>94</v>
+      </c>
       <c r="AA81" s="11"/>
       <c r="AB81" s="15"/>
       <c r="AC81" s="11"/>
@@ -7960,14 +8704,14 @@
       <c r="C82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D82" s="28" t="s">
+      <c r="D82" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
-      <c r="G82" s="29"/>
-      <c r="H82" s="29"/>
-      <c r="I82" s="30"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="39"/>
+      <c r="I82" s="41"/>
       <c r="J82" s="11"/>
       <c r="K82" s="11"/>
       <c r="L82" s="12"/>
@@ -8037,14 +8781,14 @@
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="26" t="s">
+      <c r="D83" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="27"/>
-      <c r="I83" s="31"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="45"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11"/>
       <c r="L83" s="12"/>
@@ -8483,12 +9227,78 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="AW2:AY3"/>
-    <mergeCell ref="AZ2:BE2"/>
-    <mergeCell ref="BF2:BK2"/>
-    <mergeCell ref="BL2:BQ2"/>
-    <mergeCell ref="AZ1:BQ1"/>
-    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="D56:I56"/>
+    <mergeCell ref="D57:I57"/>
+    <mergeCell ref="D77:I77"/>
+    <mergeCell ref="D71:I71"/>
+    <mergeCell ref="D78:I78"/>
+    <mergeCell ref="D80:I80"/>
+    <mergeCell ref="D81:I81"/>
+    <mergeCell ref="D82:I82"/>
+    <mergeCell ref="D75:I75"/>
+    <mergeCell ref="D76:I76"/>
+    <mergeCell ref="D72:I72"/>
+    <mergeCell ref="D73:I73"/>
+    <mergeCell ref="AK31:AP31"/>
+    <mergeCell ref="AK32:AP32"/>
+    <mergeCell ref="G66:L66"/>
+    <mergeCell ref="G67:L67"/>
+    <mergeCell ref="G60:L60"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="AK51:AP51"/>
+    <mergeCell ref="P47:X47"/>
+    <mergeCell ref="P48:X48"/>
+    <mergeCell ref="D62:I62"/>
+    <mergeCell ref="G54:L54"/>
+    <mergeCell ref="G55:L55"/>
+    <mergeCell ref="AZ21:BE21"/>
+    <mergeCell ref="AZ50:BE50"/>
+    <mergeCell ref="BF5:BK5"/>
+    <mergeCell ref="BF6:BK6"/>
+    <mergeCell ref="BF40:BK40"/>
+    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="G51:L51"/>
+    <mergeCell ref="G52:L52"/>
+    <mergeCell ref="D42:I42"/>
+    <mergeCell ref="D43:I43"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D41:O41"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="D32:O32"/>
+    <mergeCell ref="D36:I36"/>
+    <mergeCell ref="D37:I37"/>
+    <mergeCell ref="D45:I45"/>
+    <mergeCell ref="D46:I46"/>
+    <mergeCell ref="P26:X26"/>
+    <mergeCell ref="P27:X27"/>
+    <mergeCell ref="P36:X36"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="D11:O11"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D16:O16"/>
+    <mergeCell ref="D17:O17"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:X1"/>
+    <mergeCell ref="Y1:AG1"/>
+    <mergeCell ref="AH1:AP1"/>
+    <mergeCell ref="AQ1:AY1"/>
+    <mergeCell ref="AK2:AM3"/>
+    <mergeCell ref="AN2:AP3"/>
+    <mergeCell ref="AQ2:AS3"/>
+    <mergeCell ref="AT2:AV3"/>
+    <mergeCell ref="AE2:AG3"/>
+    <mergeCell ref="AH2:AJ3"/>
     <mergeCell ref="BU3:BW3"/>
     <mergeCell ref="D2:F3"/>
     <mergeCell ref="G2:I3"/>
@@ -8505,78 +9315,12 @@
     <mergeCell ref="BL3:BN3"/>
     <mergeCell ref="BO3:BQ3"/>
     <mergeCell ref="BR3:BT3"/>
-    <mergeCell ref="AK2:AM3"/>
-    <mergeCell ref="AN2:AP3"/>
-    <mergeCell ref="AQ2:AS3"/>
-    <mergeCell ref="AT2:AV3"/>
-    <mergeCell ref="AE2:AG3"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="P1:X1"/>
-    <mergeCell ref="Y1:AG1"/>
-    <mergeCell ref="AH1:AP1"/>
-    <mergeCell ref="AQ1:AY1"/>
-    <mergeCell ref="P26:X26"/>
-    <mergeCell ref="P27:X27"/>
-    <mergeCell ref="P36:X36"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D34:I34"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="D17:O17"/>
-    <mergeCell ref="D10:O10"/>
-    <mergeCell ref="G51:L51"/>
-    <mergeCell ref="G52:L52"/>
-    <mergeCell ref="D42:I42"/>
-    <mergeCell ref="D43:I43"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="D40:O40"/>
-    <mergeCell ref="D41:O41"/>
-    <mergeCell ref="D31:O31"/>
-    <mergeCell ref="D32:O32"/>
-    <mergeCell ref="D36:I36"/>
-    <mergeCell ref="D37:I37"/>
-    <mergeCell ref="AZ21:BE21"/>
-    <mergeCell ref="AZ50:BE50"/>
-    <mergeCell ref="BF5:BK5"/>
-    <mergeCell ref="BF6:BK6"/>
-    <mergeCell ref="BF40:BK40"/>
-    <mergeCell ref="D45:I45"/>
-    <mergeCell ref="D46:I46"/>
-    <mergeCell ref="D72:I72"/>
-    <mergeCell ref="D73:I73"/>
-    <mergeCell ref="AK31:AP31"/>
-    <mergeCell ref="AK32:AP32"/>
-    <mergeCell ref="G66:L66"/>
-    <mergeCell ref="G67:L67"/>
-    <mergeCell ref="G60:L60"/>
-    <mergeCell ref="G61:L61"/>
-    <mergeCell ref="AK51:AP51"/>
-    <mergeCell ref="P47:X47"/>
-    <mergeCell ref="P48:X48"/>
-    <mergeCell ref="D62:I62"/>
-    <mergeCell ref="G54:L54"/>
-    <mergeCell ref="G55:L55"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="D56:I56"/>
-    <mergeCell ref="D57:I57"/>
-    <mergeCell ref="D77:I77"/>
-    <mergeCell ref="D71:I71"/>
-    <mergeCell ref="D78:I78"/>
-    <mergeCell ref="D80:I80"/>
-    <mergeCell ref="D81:I81"/>
-    <mergeCell ref="D82:I82"/>
-    <mergeCell ref="D75:I75"/>
-    <mergeCell ref="D76:I76"/>
+    <mergeCell ref="AW2:AY3"/>
+    <mergeCell ref="AZ2:BE2"/>
+    <mergeCell ref="BF2:BK2"/>
+    <mergeCell ref="BL2:BQ2"/>
+    <mergeCell ref="AZ1:BQ1"/>
+    <mergeCell ref="AZ3:BB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Salyuk M.R. subjects
</commit_message>
<xml_diff>
--- a/Rozklad_2zaizd.xlsx
+++ b/Rozklad_2zaizd.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="240" windowWidth="20730" windowHeight="11520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="S29" authorId="0">
+    <comment ref="S29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S30" authorId="0">
+    <comment ref="S30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S59" authorId="0">
+    <comment ref="S59" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="273">
   <si>
     <t>І</t>
   </si>
@@ -725,9 +725,6 @@
     <t>Геологія загальна та історична, доц Микита М.М. (іспит)</t>
   </si>
   <si>
-    <t>Геологія загальна та історична, доц. Микита М.М. з 10:00 344 2 пари</t>
-  </si>
-  <si>
     <t>Економіка та географія природокористування</t>
   </si>
   <si>
@@ -897,13 +894,19 @@
   </si>
   <si>
     <t>Державний земельний кадастр</t>
+  </si>
+  <si>
+    <t>Геологія загальна та історична, доц. Микита М.М. з 12:00 344 2 пари</t>
+  </si>
+  <si>
+    <t>Грунтознавство (залік)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,8 +927,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -941,6 +950,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1141,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1230,6 +1251,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1284,16 +1317,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1356,7 +1401,7 @@
     </a:clrScheme>
     <a:fontScheme name="Офіс">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1391,7 +1436,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1568,7 +1613,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1579,10 +1624,10 @@
   <dimension ref="A1:BW90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="W4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AU12" sqref="AU12:AU13"/>
+      <selection pane="bottomRight" activeCell="P58" sqref="P58:Q58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,277 +1711,277 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="43" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="43" t="s">
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="43" t="s">
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="45"/>
-      <c r="AQ1" s="43" t="s">
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="49"/>
+      <c r="AQ1" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
-      <c r="AW1" s="44"/>
-      <c r="AX1" s="44"/>
-      <c r="AY1" s="45"/>
-      <c r="AZ1" s="43" t="s">
+      <c r="AR1" s="48"/>
+      <c r="AS1" s="48"/>
+      <c r="AT1" s="48"/>
+      <c r="AU1" s="48"/>
+      <c r="AV1" s="48"/>
+      <c r="AW1" s="48"/>
+      <c r="AX1" s="48"/>
+      <c r="AY1" s="49"/>
+      <c r="AZ1" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BE1" s="44"/>
-      <c r="BF1" s="44"/>
-      <c r="BG1" s="44"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
-      <c r="BL1" s="44"/>
-      <c r="BM1" s="44"/>
-      <c r="BN1" s="44"/>
-      <c r="BO1" s="44"/>
-      <c r="BP1" s="44"/>
-      <c r="BQ1" s="45"/>
+      <c r="BA1" s="48"/>
+      <c r="BB1" s="48"/>
+      <c r="BC1" s="48"/>
+      <c r="BD1" s="48"/>
+      <c r="BE1" s="48"/>
+      <c r="BF1" s="48"/>
+      <c r="BG1" s="48"/>
+      <c r="BH1" s="48"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="48"/>
+      <c r="BK1" s="48"/>
+      <c r="BL1" s="48"/>
+      <c r="BM1" s="48"/>
+      <c r="BN1" s="48"/>
+      <c r="BO1" s="48"/>
+      <c r="BP1" s="48"/>
+      <c r="BQ1" s="49"/>
     </row>
     <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="39" t="s">
+      <c r="E2" s="43"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="39" t="s">
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="39" t="s">
+      <c r="K2" s="43"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="39"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="41" t="s">
+      <c r="N2" s="43"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="39" t="s">
+      <c r="Q2" s="43"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="39"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="39" t="s">
+      <c r="T2" s="43"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="39"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="41" t="s">
+      <c r="W2" s="43"/>
+      <c r="X2" s="46"/>
+      <c r="Y2" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="39" t="s">
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="39" t="s">
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="42"/>
-      <c r="AH2" s="41" t="s">
+      <c r="AF2" s="43"/>
+      <c r="AG2" s="46"/>
+      <c r="AH2" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="40"/>
-      <c r="AK2" s="39" t="s">
+      <c r="AI2" s="43"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="40"/>
-      <c r="AN2" s="39" t="s">
+      <c r="AL2" s="43"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="42"/>
-      <c r="AQ2" s="41" t="s">
+      <c r="AO2" s="43"/>
+      <c r="AP2" s="46"/>
+      <c r="AQ2" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="AR2" s="39"/>
-      <c r="AS2" s="40"/>
-      <c r="AT2" s="39" t="s">
+      <c r="AR2" s="43"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="AU2" s="39"/>
-      <c r="AV2" s="40"/>
-      <c r="AW2" s="39" t="s">
+      <c r="AU2" s="43"/>
+      <c r="AV2" s="44"/>
+      <c r="AW2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="39"/>
-      <c r="AY2" s="42"/>
-      <c r="AZ2" s="41" t="s">
+      <c r="AX2" s="43"/>
+      <c r="AY2" s="46"/>
+      <c r="AZ2" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="BA2" s="39"/>
-      <c r="BB2" s="39"/>
-      <c r="BC2" s="39"/>
-      <c r="BD2" s="39"/>
-      <c r="BE2" s="40"/>
-      <c r="BF2" s="38" t="s">
+      <c r="BA2" s="43"/>
+      <c r="BB2" s="43"/>
+      <c r="BC2" s="43"/>
+      <c r="BD2" s="43"/>
+      <c r="BE2" s="44"/>
+      <c r="BF2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="BG2" s="39"/>
-      <c r="BH2" s="39"/>
-      <c r="BI2" s="39"/>
-      <c r="BJ2" s="39"/>
-      <c r="BK2" s="40"/>
-      <c r="BL2" s="39" t="s">
+      <c r="BG2" s="43"/>
+      <c r="BH2" s="43"/>
+      <c r="BI2" s="43"/>
+      <c r="BJ2" s="43"/>
+      <c r="BK2" s="44"/>
+      <c r="BL2" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="BM2" s="39"/>
-      <c r="BN2" s="39"/>
-      <c r="BO2" s="39"/>
-      <c r="BP2" s="39"/>
-      <c r="BQ2" s="42"/>
+      <c r="BM2" s="43"/>
+      <c r="BN2" s="43"/>
+      <c r="BO2" s="43"/>
+      <c r="BP2" s="43"/>
+      <c r="BQ2" s="46"/>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="40"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="39"/>
-      <c r="AD3" s="40"/>
-      <c r="AE3" s="39"/>
-      <c r="AF3" s="39"/>
-      <c r="AG3" s="42"/>
-      <c r="AH3" s="41"/>
-      <c r="AI3" s="39"/>
-      <c r="AJ3" s="40"/>
-      <c r="AK3" s="39"/>
-      <c r="AL3" s="39"/>
-      <c r="AM3" s="40"/>
-      <c r="AN3" s="39"/>
-      <c r="AO3" s="39"/>
-      <c r="AP3" s="42"/>
-      <c r="AQ3" s="41"/>
-      <c r="AR3" s="39"/>
-      <c r="AS3" s="40"/>
-      <c r="AT3" s="39"/>
-      <c r="AU3" s="39"/>
-      <c r="AV3" s="40"/>
-      <c r="AW3" s="39"/>
-      <c r="AX3" s="39"/>
-      <c r="AY3" s="42"/>
-      <c r="AZ3" s="41" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="46"/>
+      <c r="AH3" s="45"/>
+      <c r="AI3" s="43"/>
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="43"/>
+      <c r="AL3" s="43"/>
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="43"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="46"/>
+      <c r="AQ3" s="45"/>
+      <c r="AR3" s="43"/>
+      <c r="AS3" s="44"/>
+      <c r="AT3" s="43"/>
+      <c r="AU3" s="43"/>
+      <c r="AV3" s="44"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="43"/>
+      <c r="AY3" s="46"/>
+      <c r="AZ3" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="BA3" s="39"/>
-      <c r="BB3" s="47"/>
-      <c r="BC3" s="39" t="s">
+      <c r="BA3" s="43"/>
+      <c r="BB3" s="51"/>
+      <c r="BC3" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BD3" s="39"/>
-      <c r="BE3" s="40"/>
-      <c r="BF3" s="38" t="s">
+      <c r="BD3" s="43"/>
+      <c r="BE3" s="44"/>
+      <c r="BF3" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="BG3" s="39"/>
-      <c r="BH3" s="47"/>
-      <c r="BI3" s="39" t="s">
+      <c r="BG3" s="43"/>
+      <c r="BH3" s="51"/>
+      <c r="BI3" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="BJ3" s="39"/>
-      <c r="BK3" s="40"/>
-      <c r="BL3" s="39"/>
-      <c r="BM3" s="39"/>
-      <c r="BN3" s="47"/>
-      <c r="BO3" s="39" t="s">
+      <c r="BJ3" s="43"/>
+      <c r="BK3" s="44"/>
+      <c r="BL3" s="43"/>
+      <c r="BM3" s="43"/>
+      <c r="BN3" s="51"/>
+      <c r="BO3" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="BP3" s="39"/>
-      <c r="BQ3" s="42"/>
-      <c r="BR3" s="46"/>
-      <c r="BS3" s="46"/>
-      <c r="BT3" s="46"/>
-      <c r="BU3" s="46"/>
-      <c r="BV3" s="46"/>
-      <c r="BW3" s="46"/>
+      <c r="BP3" s="43"/>
+      <c r="BQ3" s="46"/>
+      <c r="BR3" s="50"/>
+      <c r="BS3" s="50"/>
+      <c r="BT3" s="50"/>
+      <c r="BU3" s="50"/>
+      <c r="BV3" s="50"/>
+      <c r="BW3" s="50"/>
     </row>
     <row r="4" spans="1:75" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2154,14 +2199,14 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="40"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="4" t="s">
@@ -2214,7 +2259,7 @@
       </c>
       <c r="AG5" s="6"/>
       <c r="AH5" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AI5" s="4" t="s">
         <v>188</v>
@@ -2231,7 +2276,7 @@
       </c>
       <c r="AP5" s="6"/>
       <c r="AQ5" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AR5" s="4" t="s">
         <v>179</v>
@@ -2251,14 +2296,14 @@
       <c r="BC5" s="4"/>
       <c r="BD5" s="4"/>
       <c r="BE5" s="5"/>
-      <c r="BF5" s="38" t="s">
+      <c r="BF5" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="BG5" s="39"/>
-      <c r="BH5" s="39"/>
-      <c r="BI5" s="39"/>
-      <c r="BJ5" s="39"/>
-      <c r="BK5" s="40"/>
+      <c r="BG5" s="43"/>
+      <c r="BH5" s="43"/>
+      <c r="BI5" s="43"/>
+      <c r="BJ5" s="43"/>
+      <c r="BK5" s="44"/>
       <c r="BL5" s="11"/>
       <c r="BM5" s="11"/>
       <c r="BN5" s="13"/>
@@ -2274,14 +2319,14 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
@@ -2333,7 +2378,7 @@
       <c r="AF6" s="4"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AI6" s="4" t="s">
         <v>188</v>
@@ -2352,7 +2397,7 @@
       </c>
       <c r="AP6" s="6"/>
       <c r="AQ6" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AR6" s="4" t="s">
         <v>179</v>
@@ -2372,14 +2417,14 @@
       <c r="BC6" s="4"/>
       <c r="BD6" s="4"/>
       <c r="BE6" s="5"/>
-      <c r="BF6" s="38" t="s">
+      <c r="BF6" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="BG6" s="39"/>
-      <c r="BH6" s="39"/>
-      <c r="BI6" s="39"/>
-      <c r="BJ6" s="39"/>
-      <c r="BK6" s="40"/>
+      <c r="BG6" s="43"/>
+      <c r="BH6" s="43"/>
+      <c r="BI6" s="43"/>
+      <c r="BJ6" s="43"/>
+      <c r="BK6" s="44"/>
       <c r="BL6" s="11"/>
       <c r="BM6" s="11"/>
       <c r="BN6" s="13"/>
@@ -2395,14 +2440,14 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="40"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="5"/>
@@ -2462,7 +2507,7 @@
       <c r="AL7" s="4"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AO7" s="4" t="s">
         <v>144</v>
@@ -2506,20 +2551,20 @@
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="42"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="46"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="5"/>
@@ -2557,7 +2602,7 @@
       <c r="AL8" s="4"/>
       <c r="AM8" s="5"/>
       <c r="AN8" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AO8" s="11" t="s">
         <v>101</v>
@@ -2669,24 +2714,24 @@
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="9" t="s">
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="Q10" s="11" t="s">
+      <c r="Q10" s="55" t="s">
         <v>114</v>
       </c>
       <c r="R10" s="12"/>
@@ -2729,21 +2774,21 @@
       <c r="AI10" s="11"/>
       <c r="AJ10" s="12"/>
       <c r="AK10" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AL10" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="AL10" s="11" t="s">
-        <v>236</v>
       </c>
       <c r="AM10" s="12"/>
       <c r="AN10" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AO10" s="11" t="s">
         <v>101</v>
       </c>
       <c r="AP10" s="14"/>
       <c r="AQ10" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AR10" s="11" t="s">
         <v>179</v>
@@ -2782,24 +2827,24 @@
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="9" t="s">
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="Q11" s="11" t="s">
+      <c r="Q11" s="55" t="s">
         <v>114</v>
       </c>
       <c r="R11" s="12"/>
@@ -2839,28 +2884,28 @@
       </c>
       <c r="AG11" s="14"/>
       <c r="AH11" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AI11" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AJ11" s="12"/>
       <c r="AK11" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AL11" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="AL11" s="11" t="s">
-        <v>236</v>
       </c>
       <c r="AM11" s="12"/>
       <c r="AN11" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AO11" s="11" t="s">
         <v>101</v>
       </c>
       <c r="AP11" s="14"/>
       <c r="AQ11" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AR11" s="10" t="s">
         <v>179</v>
@@ -2901,14 +2946,14 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="35"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="12"/>
@@ -2926,10 +2971,10 @@
         <v>125</v>
       </c>
       <c r="R12" s="12"/>
-      <c r="S12" s="11" t="s">
+      <c r="S12" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="T12" s="11" t="s">
+      <c r="T12" s="55" t="s">
         <v>114</v>
       </c>
       <c r="U12" s="12"/>
@@ -2962,7 +3007,7 @@
       </c>
       <c r="AG12" s="14"/>
       <c r="AH12" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AI12" s="11" t="s">
         <v>171</v>
@@ -2972,7 +3017,7 @@
       <c r="AL12" s="11"/>
       <c r="AM12" s="12"/>
       <c r="AN12" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AO12" s="11" t="s">
         <v>210</v>
@@ -2982,7 +3027,7 @@
       <c r="AR12" s="11"/>
       <c r="AS12" s="12"/>
       <c r="AT12" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AU12" s="11" t="s">
         <v>137</v>
@@ -3020,14 +3065,14 @@
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="12"/>
@@ -3041,10 +3086,10 @@
         <v>125</v>
       </c>
       <c r="R13" s="12"/>
-      <c r="S13" s="11" t="s">
+      <c r="S13" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="T13" s="11" t="s">
+      <c r="T13" s="55" t="s">
         <v>114</v>
       </c>
       <c r="U13" s="12"/>
@@ -3083,7 +3128,7 @@
       <c r="AL13" s="11"/>
       <c r="AM13" s="12"/>
       <c r="AN13" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AO13" s="11" t="s">
         <v>210</v>
@@ -3093,7 +3138,7 @@
       <c r="AR13" s="11"/>
       <c r="AS13" s="12"/>
       <c r="AT13" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AU13" s="11" t="s">
         <v>137</v>
@@ -3121,7 +3166,7 @@
       <c r="BP13" s="11"/>
       <c r="BQ13" s="14"/>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75" ht="60" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
         <v>75</v>
       </c>
@@ -3146,6 +3191,12 @@
       <c r="V14" s="11"/>
       <c r="W14" s="11"/>
       <c r="X14" s="14"/>
+      <c r="Y14" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z14" s="26" t="s">
+        <v>93</v>
+      </c>
       <c r="AA14" s="12"/>
       <c r="AB14" s="11"/>
       <c r="AC14" s="11"/>
@@ -3221,7 +3272,7 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="14"/>
-      <c r="Y15" s="27" t="s">
+      <c r="Y15" s="29" t="s">
         <v>161</v>
       </c>
       <c r="Z15" s="26" t="s">
@@ -3240,13 +3291,13 @@
       <c r="AI15" s="11"/>
       <c r="AJ15" s="12"/>
       <c r="AK15" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AL15" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="AM15" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="AL15" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="AM15" s="12" t="s">
-        <v>231</v>
       </c>
       <c r="AN15" s="11" t="s">
         <v>202</v>
@@ -3290,20 +3341,20 @@
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="41"/>
       <c r="P16" s="9" t="s">
         <v>58</v>
       </c>
@@ -3328,7 +3379,7 @@
       <c r="Y16" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="Z16" s="26" t="s">
+      <c r="Z16" s="11" t="s">
         <v>93</v>
       </c>
       <c r="AA16" s="12"/>
@@ -3352,30 +3403,30 @@
       <c r="AI16" s="11"/>
       <c r="AJ16" s="12"/>
       <c r="AK16" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="AL16" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="AM16" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="AL16" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="AM16" s="12" t="s">
-        <v>231</v>
-      </c>
       <c r="AN16" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AO16" s="11" t="s">
         <v>210</v>
       </c>
       <c r="AP16" s="14"/>
       <c r="AQ16" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AR16" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AS16" s="12"/>
       <c r="AT16" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AU16" s="11" t="s">
         <v>183</v>
@@ -3411,20 +3462,20 @@
       <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="41"/>
       <c r="P17" s="9" t="s">
         <v>58</v>
       </c>
@@ -3446,8 +3497,8 @@
         <v>155</v>
       </c>
       <c r="X17" s="14"/>
-      <c r="Y17" s="29" t="s">
-        <v>161</v>
+      <c r="Y17" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="Z17" s="11" t="s">
         <v>93</v>
@@ -3468,35 +3519,35 @@
       </c>
       <c r="AG17" s="14"/>
       <c r="AH17" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI17" s="11" t="s">
         <v>195</v>
       </c>
       <c r="AJ17" s="12"/>
       <c r="AK17" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL17" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="AL17" s="11" t="s">
-        <v>234</v>
       </c>
       <c r="AM17" s="12"/>
       <c r="AN17" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AO17" s="11" t="s">
         <v>210</v>
       </c>
       <c r="AP17" s="14"/>
       <c r="AQ17" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AR17" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AS17" s="12"/>
       <c r="AT17" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AU17" s="11" t="s">
         <v>183</v>
@@ -3524,7 +3575,7 @@
       <c r="BP17" s="11"/>
       <c r="BQ17" s="14"/>
     </row>
-    <row r="18" spans="1:69" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:69" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>3</v>
@@ -3553,12 +3604,6 @@
       <c r="V18" s="11"/>
       <c r="W18" s="11"/>
       <c r="X18" s="14"/>
-      <c r="Y18" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="Z18" s="11" t="s">
-        <v>93</v>
-      </c>
       <c r="AA18" s="12"/>
       <c r="AB18" s="11"/>
       <c r="AC18" s="11"/>
@@ -3570,10 +3615,10 @@
       <c r="AI18" s="11"/>
       <c r="AJ18" s="12"/>
       <c r="AK18" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL18" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="AL18" s="11" t="s">
-        <v>234</v>
       </c>
       <c r="AM18" s="12"/>
       <c r="AN18" s="11"/>
@@ -3764,14 +3809,14 @@
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="12"/>
@@ -3823,17 +3868,17 @@
       </c>
       <c r="AG21" s="14"/>
       <c r="AH21" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI21" s="11" t="s">
         <v>195</v>
       </c>
       <c r="AJ21" s="12"/>
       <c r="AK21" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AL21" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="AL21" s="11" t="s">
-        <v>236</v>
       </c>
       <c r="AM21" s="12"/>
       <c r="AN21" s="11" t="s">
@@ -3844,7 +3889,7 @@
       </c>
       <c r="AP21" s="14"/>
       <c r="AQ21" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AR21" s="11" t="s">
         <v>179</v>
@@ -3856,14 +3901,14 @@
       <c r="AW21" s="11"/>
       <c r="AX21" s="11"/>
       <c r="AY21" s="14"/>
-      <c r="AZ21" s="33" t="s">
+      <c r="AZ21" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="BA21" s="34"/>
-      <c r="BB21" s="34"/>
-      <c r="BC21" s="34"/>
-      <c r="BD21" s="34"/>
-      <c r="BE21" s="35"/>
+      <c r="BA21" s="38"/>
+      <c r="BB21" s="38"/>
+      <c r="BC21" s="38"/>
+      <c r="BD21" s="38"/>
+      <c r="BE21" s="39"/>
       <c r="BF21" s="11"/>
       <c r="BG21" s="11"/>
       <c r="BH21" s="13"/>
@@ -3885,14 +3930,14 @@
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="35"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="12"/>
@@ -3944,17 +3989,17 @@
       </c>
       <c r="AG22" s="14"/>
       <c r="AH22" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AI22" s="11" t="s">
         <v>195</v>
       </c>
       <c r="AJ22" s="12"/>
       <c r="AK22" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AL22" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="AL22" s="11" t="s">
-        <v>236</v>
       </c>
       <c r="AM22" s="12"/>
       <c r="AN22" s="11" t="s">
@@ -3965,7 +4010,7 @@
       </c>
       <c r="AP22" s="14"/>
       <c r="AQ22" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AR22" s="11" t="s">
         <v>179</v>
@@ -3977,12 +4022,6 @@
       <c r="AW22" s="11"/>
       <c r="AX22" s="11"/>
       <c r="AY22" s="14"/>
-      <c r="AZ22" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="BA22" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="BB22" s="13"/>
       <c r="BC22" s="11"/>
       <c r="BD22" s="11"/>
@@ -4048,7 +4087,7 @@
       <c r="AL23" s="11"/>
       <c r="AM23" s="12"/>
       <c r="AN23" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AO23" s="28" t="s">
         <v>144</v>
@@ -4063,12 +4102,6 @@
       <c r="AW23" s="11"/>
       <c r="AX23" s="11"/>
       <c r="AY23" s="14"/>
-      <c r="AZ23" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="BA23" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="BB23" s="13"/>
       <c r="BC23" s="11"/>
       <c r="BD23" s="11"/>
@@ -4164,20 +4197,20 @@
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="37"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="41"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="12"/>
@@ -4241,14 +4274,14 @@
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="35"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="39"/>
       <c r="J26" s="11" t="s">
         <v>91</v>
       </c>
@@ -4263,23 +4296,17 @@
         <v>63</v>
       </c>
       <c r="O26" s="14"/>
-      <c r="P26" s="33" t="s">
+      <c r="P26" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="34"/>
-      <c r="W26" s="34"/>
-      <c r="X26" s="37"/>
-      <c r="Y26" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z26" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="41"/>
       <c r="AA26" s="12"/>
       <c r="AB26" s="15" t="s">
         <v>67</v>
@@ -4294,28 +4321,28 @@
       </c>
       <c r="AG26" s="14"/>
       <c r="AH26" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AI26" s="11" t="s">
         <v>171</v>
       </c>
       <c r="AJ26" s="12"/>
-      <c r="AK26" s="48" t="s">
+      <c r="AK26" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="AL26" s="30" t="s">
         <v>228</v>
-      </c>
-      <c r="AL26" s="48" t="s">
-        <v>229</v>
       </c>
       <c r="AM26" s="12"/>
       <c r="AN26" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AO26" s="11" t="s">
         <v>210</v>
       </c>
       <c r="AP26" s="14"/>
       <c r="AQ26" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AR26" s="11" t="s">
         <v>179</v>
@@ -4356,14 +4383,14 @@
       <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="35"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="39"/>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
       <c r="L27" s="12"/>
@@ -4374,21 +4401,21 @@
         <v>63</v>
       </c>
       <c r="O27" s="14"/>
-      <c r="P27" s="33" t="s">
+      <c r="P27" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="34"/>
-      <c r="T27" s="34"/>
-      <c r="U27" s="34"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="34"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="9" t="s">
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="Z27" s="11" t="s">
+      <c r="Z27" s="55" t="s">
         <v>114</v>
       </c>
       <c r="AA27" s="12"/>
@@ -4407,28 +4434,28 @@
       </c>
       <c r="AG27" s="14"/>
       <c r="AH27" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AI27" s="11" t="s">
         <v>171</v>
       </c>
       <c r="AJ27" s="12"/>
-      <c r="AK27" s="48" t="s">
+      <c r="AK27" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="AL27" s="30" t="s">
         <v>228</v>
-      </c>
-      <c r="AL27" s="48" t="s">
-        <v>229</v>
       </c>
       <c r="AM27" s="12"/>
       <c r="AN27" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AO27" s="11" t="s">
         <v>210</v>
       </c>
       <c r="AP27" s="14"/>
       <c r="AQ27" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AR27" s="11" t="s">
         <v>179</v>
@@ -4459,7 +4486,7 @@
       <c r="BP27" s="11"/>
       <c r="BQ27" s="14"/>
     </row>
-    <row r="28" spans="1:69" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:69" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>3</v>
@@ -4488,8 +4515,12 @@
       <c r="V28" s="11"/>
       <c r="W28" s="11"/>
       <c r="X28" s="14"/>
-      <c r="Y28" s="9"/>
-      <c r="Z28" s="11"/>
+      <c r="Y28" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z28" s="55" t="s">
+        <v>114</v>
+      </c>
       <c r="AA28" s="12"/>
       <c r="AB28" s="11" t="s">
         <v>193</v>
@@ -4539,14 +4570,14 @@
       <c r="BQ28" s="14"/>
     </row>
     <row r="29" spans="1:69" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32"/>
+      <c r="D29" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="36"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
       <c r="L29" s="12"/>
@@ -4658,7 +4689,7 @@
       <c r="AO30" s="11"/>
       <c r="AP30" s="14"/>
       <c r="AQ30" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AR30" s="11" t="s">
         <v>195</v>
@@ -4697,20 +4728,20 @@
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
-      <c r="O31" s="37"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="41"/>
       <c r="P31" s="9" t="s">
         <v>116</v>
       </c>
@@ -4754,22 +4785,22 @@
       </c>
       <c r="AG31" s="14"/>
       <c r="AH31" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AI31" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AJ31" s="12"/>
-      <c r="AK31" s="36" t="s">
+      <c r="AK31" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="AL31" s="34"/>
-      <c r="AM31" s="34"/>
-      <c r="AN31" s="34"/>
-      <c r="AO31" s="34"/>
-      <c r="AP31" s="37"/>
+      <c r="AL31" s="38"/>
+      <c r="AM31" s="38"/>
+      <c r="AN31" s="38"/>
+      <c r="AO31" s="38"/>
+      <c r="AP31" s="41"/>
       <c r="AQ31" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AR31" s="11" t="s">
         <v>195</v>
@@ -4806,20 +4837,20 @@
       <c r="C32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="37"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="41"/>
       <c r="P32" s="9" t="s">
         <v>58</v>
       </c>
@@ -4833,10 +4864,10 @@
       <c r="V32" s="11"/>
       <c r="W32" s="11"/>
       <c r="X32" s="14"/>
-      <c r="Y32" s="9" t="s">
+      <c r="Y32" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="Z32" s="11" t="s">
+      <c r="Z32" s="55" t="s">
         <v>114</v>
       </c>
       <c r="AA32" s="12"/>
@@ -4857,14 +4888,14 @@
       <c r="AH32" s="9"/>
       <c r="AI32" s="11"/>
       <c r="AJ32" s="12"/>
-      <c r="AK32" s="36" t="s">
+      <c r="AK32" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="AL32" s="34"/>
-      <c r="AM32" s="34"/>
-      <c r="AN32" s="34"/>
-      <c r="AO32" s="34"/>
-      <c r="AP32" s="37"/>
+      <c r="AL32" s="38"/>
+      <c r="AM32" s="38"/>
+      <c r="AN32" s="38"/>
+      <c r="AO32" s="38"/>
+      <c r="AP32" s="41"/>
       <c r="AQ32" s="10" t="s">
         <v>102</v>
       </c>
@@ -4924,10 +4955,10 @@
       <c r="V33" s="11"/>
       <c r="W33" s="11"/>
       <c r="X33" s="14"/>
-      <c r="Y33" s="9" t="s">
+      <c r="Y33" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="Z33" s="11" t="s">
+      <c r="Z33" s="55" t="s">
         <v>114</v>
       </c>
       <c r="AA33" s="12"/>
@@ -4978,14 +5009,14 @@
       <c r="C34" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="35"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="39"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
       <c r="L34" s="12"/>
@@ -5088,26 +5119,26 @@
       <c r="AF35" s="11"/>
       <c r="AG35" s="14"/>
       <c r="AH35" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI35" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="AI35" s="11" t="s">
-        <v>225</v>
       </c>
       <c r="AJ35" s="12"/>
       <c r="AK35" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="AL35" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="AL35" s="10" t="s">
-        <v>243</v>
       </c>
       <c r="AM35" s="12"/>
       <c r="AN35" s="11"/>
       <c r="AO35" s="11"/>
       <c r="AP35" s="14"/>
-      <c r="AQ35" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="AR35" s="11" t="s">
+      <c r="AQ35" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="AR35" s="55" t="s">
         <v>114</v>
       </c>
       <c r="AS35" s="12"/>
@@ -5144,14 +5175,14 @@
       <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="35"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="39"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="12"/>
@@ -5162,17 +5193,17 @@
         <v>63</v>
       </c>
       <c r="O36" s="14"/>
-      <c r="P36" s="33" t="s">
+      <c r="P36" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="34"/>
-      <c r="W36" s="34"/>
-      <c r="X36" s="37"/>
+      <c r="Q36" s="38"/>
+      <c r="R36" s="38"/>
+      <c r="S36" s="38"/>
+      <c r="T36" s="38"/>
+      <c r="U36" s="38"/>
+      <c r="V36" s="38"/>
+      <c r="W36" s="38"/>
+      <c r="X36" s="41"/>
       <c r="Y36" s="9" t="s">
         <v>79</v>
       </c>
@@ -5193,7 +5224,7 @@
       </c>
       <c r="AG36" s="14"/>
       <c r="AH36" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI36" s="11" t="s">
         <v>173</v>
@@ -5203,10 +5234,10 @@
       <c r="AN36" s="11"/>
       <c r="AO36" s="11"/>
       <c r="AP36" s="14"/>
-      <c r="AQ36" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="AR36" s="11" t="s">
+      <c r="AQ36" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="AR36" s="55" t="s">
         <v>114</v>
       </c>
       <c r="AS36" s="12"/>
@@ -5243,14 +5274,14 @@
       <c r="C37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="39"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="12"/>
@@ -5294,7 +5325,7 @@
       </c>
       <c r="AG37" s="14"/>
       <c r="AH37" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI37" s="11" t="s">
         <v>173</v>
@@ -5302,7 +5333,7 @@
       <c r="AJ37" s="12"/>
       <c r="AM37" s="12"/>
       <c r="AN37" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AO37" s="28" t="s">
         <v>144</v>
@@ -5317,8 +5348,8 @@
       <c r="AW37" s="11"/>
       <c r="AX37" s="11"/>
       <c r="AY37" s="14"/>
-      <c r="AZ37" s="9"/>
-      <c r="BA37" s="11"/>
+      <c r="AZ37" s="56"/>
+      <c r="BA37" s="58"/>
       <c r="BB37" s="13"/>
       <c r="BC37" s="11"/>
       <c r="BD37" s="11"/>
@@ -5393,7 +5424,7 @@
       <c r="AL38" s="11"/>
       <c r="AM38" s="12"/>
       <c r="AN38" s="28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AO38" s="28" t="s">
         <v>144</v>
@@ -5408,8 +5439,8 @@
       <c r="AW38" s="11"/>
       <c r="AX38" s="11"/>
       <c r="AY38" s="14"/>
-      <c r="AZ38" s="9"/>
-      <c r="BA38" s="11"/>
+      <c r="AZ38" s="56"/>
+      <c r="BA38" s="58"/>
       <c r="BB38" s="13"/>
       <c r="BC38" s="11"/>
       <c r="BD38" s="11"/>
@@ -5505,20 +5536,20 @@
       <c r="C40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="39"/>
-      <c r="N40" s="39"/>
-      <c r="O40" s="42"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="46"/>
       <c r="P40" s="9" t="s">
         <v>124</v>
       </c>
@@ -5563,23 +5594,23 @@
       <c r="AI40" s="11"/>
       <c r="AJ40" s="12"/>
       <c r="AK40" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL40" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="AL40" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="AM40" s="12"/>
       <c r="AN40" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AO40" s="11" t="s">
         <v>210</v>
       </c>
       <c r="AP40" s="14"/>
-      <c r="AQ40" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="AR40" s="11" t="s">
+      <c r="AQ40" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="AR40" s="55" t="s">
         <v>114</v>
       </c>
       <c r="AS40" s="12"/>
@@ -5595,14 +5626,14 @@
       <c r="BC40" s="11"/>
       <c r="BD40" s="11"/>
       <c r="BE40" s="12"/>
-      <c r="BF40" s="38" t="s">
+      <c r="BF40" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="BG40" s="39"/>
-      <c r="BH40" s="39"/>
-      <c r="BI40" s="39"/>
-      <c r="BJ40" s="39"/>
-      <c r="BK40" s="40"/>
+      <c r="BG40" s="43"/>
+      <c r="BH40" s="43"/>
+      <c r="BI40" s="43"/>
+      <c r="BJ40" s="43"/>
+      <c r="BK40" s="44"/>
       <c r="BL40" s="11"/>
       <c r="BM40" s="11"/>
       <c r="BN40" s="13"/>
@@ -5618,20 +5649,20 @@
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="41" t="s">
+      <c r="D41" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
-      <c r="O41" s="42"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="46"/>
       <c r="P41" s="9" t="s">
         <v>124</v>
       </c>
@@ -5676,23 +5707,23 @@
       <c r="AI41" s="11"/>
       <c r="AJ41" s="12"/>
       <c r="AK41" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL41" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="AL41" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="AM41" s="12"/>
       <c r="AN41" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AO41" s="11" t="s">
         <v>210</v>
       </c>
       <c r="AP41" s="14"/>
-      <c r="AQ41" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="AR41" s="11" t="s">
+      <c r="AQ41" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="AR41" s="55" t="s">
         <v>114</v>
       </c>
       <c r="AS41" s="12"/>
@@ -5728,14 +5759,14 @@
       <c r="C42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="35"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="39"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
       <c r="L42" s="12"/>
@@ -5746,10 +5777,10 @@
         <v>103</v>
       </c>
       <c r="O42" s="14"/>
-      <c r="P42" s="9" t="s">
+      <c r="P42" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="Q42" s="11" t="s">
+      <c r="Q42" s="55" t="s">
         <v>114</v>
       </c>
       <c r="R42" s="12"/>
@@ -5785,21 +5816,21 @@
       </c>
       <c r="AG42" s="14"/>
       <c r="AH42" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AI42" s="11" t="s">
         <v>121</v>
       </c>
       <c r="AJ42" s="12"/>
       <c r="AK42" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AL42" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="AL42" s="11" t="s">
-        <v>239</v>
-      </c>
       <c r="AM42" s="12"/>
-      <c r="AN42" s="51" t="s">
-        <v>258</v>
+      <c r="AN42" s="33" t="s">
+        <v>257</v>
       </c>
       <c r="AO42" s="11" t="s">
         <v>210</v>
@@ -5822,14 +5853,14 @@
       <c r="BC42" s="11"/>
       <c r="BD42" s="11"/>
       <c r="BE42" s="12"/>
-      <c r="BF42" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="BG42" s="34"/>
-      <c r="BH42" s="34"/>
-      <c r="BI42" s="34"/>
-      <c r="BJ42" s="34"/>
-      <c r="BK42" s="35"/>
+      <c r="BF42" s="40" t="s">
+        <v>245</v>
+      </c>
+      <c r="BG42" s="38"/>
+      <c r="BH42" s="38"/>
+      <c r="BI42" s="38"/>
+      <c r="BJ42" s="38"/>
+      <c r="BK42" s="39"/>
       <c r="BL42" s="11"/>
       <c r="BM42" s="11"/>
       <c r="BN42" s="13"/>
@@ -5845,14 +5876,14 @@
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="35"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="39"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
       <c r="L43" s="12"/>
@@ -5863,10 +5894,10 @@
         <v>103</v>
       </c>
       <c r="O43" s="14"/>
-      <c r="P43" s="9" t="s">
+      <c r="P43" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="Q43" s="11" t="s">
+      <c r="Q43" s="55" t="s">
         <v>114</v>
       </c>
       <c r="R43" s="12"/>
@@ -5905,8 +5936,8 @@
       <c r="AI43" s="11"/>
       <c r="AJ43" s="12"/>
       <c r="AM43" s="12"/>
-      <c r="AN43" s="51" t="s">
-        <v>258</v>
+      <c r="AN43" s="33" t="s">
+        <v>257</v>
       </c>
       <c r="AO43" s="11" t="s">
         <v>210</v>
@@ -5929,14 +5960,14 @@
       <c r="BC43" s="11"/>
       <c r="BD43" s="11"/>
       <c r="BE43" s="12"/>
-      <c r="BF43" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="BG43" s="34"/>
-      <c r="BH43" s="34"/>
-      <c r="BI43" s="34"/>
-      <c r="BJ43" s="34"/>
-      <c r="BK43" s="35"/>
+      <c r="BF43" s="40" t="s">
+        <v>245</v>
+      </c>
+      <c r="BG43" s="38"/>
+      <c r="BH43" s="38"/>
+      <c r="BI43" s="38"/>
+      <c r="BJ43" s="38"/>
+      <c r="BK43" s="39"/>
       <c r="BL43" s="11"/>
       <c r="BM43" s="11"/>
       <c r="BN43" s="13"/>
@@ -6022,14 +6053,14 @@
       <c r="C45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="32"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="36"/>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
       <c r="L45" s="12"/>
@@ -6050,10 +6081,10 @@
       <c r="S45" s="11"/>
       <c r="T45" s="11"/>
       <c r="U45" s="12"/>
-      <c r="V45" s="49" t="s">
+      <c r="V45" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="W45" s="49" t="s">
+      <c r="W45" s="31" t="s">
         <v>160</v>
       </c>
       <c r="X45" s="14"/>
@@ -6081,8 +6112,8 @@
       <c r="AH45" s="9"/>
       <c r="AI45" s="11"/>
       <c r="AJ45" s="12"/>
-      <c r="AK45" s="50"/>
-      <c r="AL45" s="50"/>
+      <c r="AK45" s="32"/>
+      <c r="AL45" s="32"/>
       <c r="AM45" s="12"/>
       <c r="AN45" s="11"/>
       <c r="AO45" s="11"/>
@@ -6123,14 +6154,14 @@
       <c r="C46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="32"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="36"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
       <c r="L46" s="12"/>
@@ -6151,10 +6182,10 @@
       <c r="S46" s="11"/>
       <c r="T46" s="11"/>
       <c r="U46" s="12"/>
-      <c r="V46" s="49" t="s">
+      <c r="V46" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="W46" s="49" t="s">
+      <c r="W46" s="31" t="s">
         <v>160</v>
       </c>
       <c r="X46" s="14"/>
@@ -6182,8 +6213,8 @@
       <c r="AH46" s="9"/>
       <c r="AI46" s="11"/>
       <c r="AJ46" s="12"/>
-      <c r="AK46" s="50"/>
-      <c r="AL46" s="50"/>
+      <c r="AK46" s="32"/>
+      <c r="AL46" s="32"/>
       <c r="AM46" s="12"/>
       <c r="AN46" s="11"/>
       <c r="AO46" s="11"/>
@@ -6228,38 +6259,38 @@
       <c r="C47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="32"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
       <c r="L47" s="12"/>
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
       <c r="O47" s="14"/>
-      <c r="P47" s="33" t="s">
+      <c r="P47" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Q47" s="34"/>
-      <c r="R47" s="34"/>
-      <c r="S47" s="34"/>
-      <c r="T47" s="34"/>
-      <c r="U47" s="34"/>
-      <c r="V47" s="34"/>
-      <c r="W47" s="34"/>
-      <c r="X47" s="37"/>
+      <c r="Q47" s="38"/>
+      <c r="R47" s="38"/>
+      <c r="S47" s="38"/>
+      <c r="T47" s="38"/>
+      <c r="U47" s="38"/>
+      <c r="V47" s="38"/>
+      <c r="W47" s="38"/>
+      <c r="X47" s="41"/>
       <c r="Y47" s="9"/>
       <c r="Z47" s="11"/>
       <c r="AA47" s="12"/>
-      <c r="AB47" s="48" t="s">
+      <c r="AB47" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="AC47" s="48" t="s">
+      <c r="AC47" s="30" t="s">
         <v>191</v>
       </c>
       <c r="AD47" s="12"/>
@@ -6271,17 +6302,17 @@
       </c>
       <c r="AG47" s="14"/>
       <c r="AH47" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AI47" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AJ47" s="12"/>
-      <c r="AK47" s="50"/>
-      <c r="AL47" s="50"/>
+      <c r="AK47" s="32"/>
+      <c r="AL47" s="32"/>
       <c r="AM47" s="12"/>
-      <c r="AN47" s="51" t="s">
-        <v>256</v>
+      <c r="AN47" s="33" t="s">
+        <v>255</v>
       </c>
       <c r="AO47" s="11" t="s">
         <v>210</v>
@@ -6323,31 +6354,31 @@
       <c r="C48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
-      <c r="I48" s="32"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="36"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
       <c r="L48" s="12"/>
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
       <c r="O48" s="14"/>
-      <c r="P48" s="33" t="s">
+      <c r="P48" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="Q48" s="34"/>
-      <c r="R48" s="34"/>
-      <c r="S48" s="34"/>
-      <c r="T48" s="34"/>
-      <c r="U48" s="34"/>
-      <c r="V48" s="34"/>
-      <c r="W48" s="34"/>
-      <c r="X48" s="37"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="38"/>
+      <c r="U48" s="38"/>
+      <c r="V48" s="38"/>
+      <c r="W48" s="38"/>
+      <c r="X48" s="41"/>
       <c r="Y48" s="11"/>
       <c r="Z48" s="11"/>
       <c r="AA48" s="11"/>
@@ -6358,21 +6389,21 @@
       <c r="AF48" s="11"/>
       <c r="AG48" s="14"/>
       <c r="AH48" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AI48" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AJ48" s="12"/>
-      <c r="AK48" s="50" t="s">
-        <v>249</v>
+      <c r="AK48" s="32" t="s">
+        <v>248</v>
       </c>
       <c r="AL48" s="11" t="s">
         <v>160</v>
       </c>
       <c r="AM48" s="12"/>
       <c r="AN48" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AO48" s="11" t="s">
         <v>210</v>
@@ -6406,7 +6437,7 @@
       <c r="BP48" s="11"/>
       <c r="BQ48" s="14"/>
     </row>
-    <row r="49" spans="1:69" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:69" ht="75" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>75</v>
       </c>
@@ -6435,8 +6466,12 @@
       <c r="V49" s="11"/>
       <c r="W49" s="11"/>
       <c r="X49" s="14"/>
-      <c r="Y49" s="11"/>
-      <c r="Z49" s="11"/>
+      <c r="Y49" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z49" s="53" t="s">
+        <v>114</v>
+      </c>
       <c r="AA49" s="11"/>
       <c r="AB49" s="15"/>
       <c r="AC49" s="11"/>
@@ -6506,8 +6541,12 @@
       <c r="N50" s="11"/>
       <c r="O50" s="14"/>
       <c r="R50" s="12"/>
-      <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
+      <c r="S50" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="T50" s="59" t="s">
+        <v>114</v>
+      </c>
       <c r="U50" s="12"/>
       <c r="V50" s="11"/>
       <c r="W50" s="11"/>
@@ -6543,14 +6582,14 @@
       <c r="AW50" s="11"/>
       <c r="AX50" s="11"/>
       <c r="AY50" s="14"/>
-      <c r="AZ50" s="33" t="s">
+      <c r="AZ50" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="BA50" s="34"/>
-      <c r="BB50" s="34"/>
-      <c r="BC50" s="34"/>
-      <c r="BD50" s="34"/>
-      <c r="BE50" s="35"/>
+      <c r="BA50" s="38"/>
+      <c r="BB50" s="38"/>
+      <c r="BC50" s="38"/>
+      <c r="BD50" s="38"/>
+      <c r="BE50" s="39"/>
       <c r="BF50" s="11"/>
       <c r="BG50" s="11"/>
       <c r="BH50" s="13"/>
@@ -6575,14 +6614,14 @@
       <c r="D51" s="9"/>
       <c r="E51" s="11"/>
       <c r="F51" s="12"/>
-      <c r="G51" s="36" t="s">
+      <c r="G51" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="35"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
+      <c r="K51" s="38"/>
+      <c r="L51" s="39"/>
       <c r="M51" s="10" t="s">
         <v>89</v>
       </c>
@@ -6635,14 +6674,14 @@
       <c r="AH51" s="11"/>
       <c r="AI51" s="11"/>
       <c r="AJ51" s="12"/>
-      <c r="AK51" s="36" t="s">
+      <c r="AK51" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="AL51" s="34"/>
-      <c r="AM51" s="34"/>
-      <c r="AN51" s="34"/>
-      <c r="AO51" s="34"/>
-      <c r="AP51" s="37"/>
+      <c r="AL51" s="38"/>
+      <c r="AM51" s="38"/>
+      <c r="AN51" s="38"/>
+      <c r="AO51" s="38"/>
+      <c r="AP51" s="41"/>
       <c r="AQ51" s="11"/>
       <c r="AR51" s="11"/>
       <c r="AS51" s="12"/>
@@ -6676,14 +6715,14 @@
       <c r="D52" s="9"/>
       <c r="E52" s="11"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="36" t="s">
+      <c r="G52" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
-      <c r="L52" s="35"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="39"/>
       <c r="M52" s="10" t="s">
         <v>89</v>
       </c>
@@ -6855,14 +6894,14 @@
       <c r="D54" s="9"/>
       <c r="E54" s="11"/>
       <c r="F54" s="12"/>
-      <c r="G54" s="36" t="s">
+      <c r="G54" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="35"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
+      <c r="L54" s="39"/>
       <c r="M54" s="11"/>
       <c r="N54" s="11"/>
       <c r="O54" s="14"/>
@@ -6934,14 +6973,14 @@
       <c r="D55" s="9"/>
       <c r="E55" s="11"/>
       <c r="F55" s="12"/>
-      <c r="G55" s="36" t="s">
+      <c r="G55" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="34"/>
-      <c r="K55" s="34"/>
-      <c r="L55" s="35"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="39"/>
       <c r="M55" s="11"/>
       <c r="N55" s="11"/>
       <c r="O55" s="14"/>
@@ -7008,14 +7047,14 @@
       <c r="C56" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D56" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
       <c r="M56" s="11" t="s">
         <v>105</v>
       </c>
@@ -7062,14 +7101,14 @@
       </c>
       <c r="AG56" s="14"/>
       <c r="AH56" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI56" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AJ56" s="12"/>
       <c r="AK56" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AL56" s="11" t="s">
         <v>195</v>
@@ -7082,7 +7121,7 @@
       <c r="AR56" s="11"/>
       <c r="AS56" s="12"/>
       <c r="AT56" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AU56" s="11" t="s">
         <v>183</v>
@@ -7118,14 +7157,14 @@
       <c r="C57" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
       <c r="M57" s="11" t="s">
         <v>105</v>
       </c>
@@ -7171,14 +7210,14 @@
       </c>
       <c r="AG57" s="14"/>
       <c r="AH57" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI57" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AJ57" s="12"/>
       <c r="AK57" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AL57" s="11" t="s">
         <v>195</v>
@@ -7188,10 +7227,10 @@
       <c r="AO57" s="11"/>
       <c r="AP57" s="14"/>
       <c r="AQ57" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="AR57" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="AR57" s="11" t="s">
-        <v>268</v>
       </c>
       <c r="AS57" s="12"/>
       <c r="AT57" s="11"/>
@@ -7219,7 +7258,7 @@
       <c r="BP57" s="11"/>
       <c r="BQ57" s="14"/>
     </row>
-    <row r="58" spans="1:69" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:69" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
         <v>3</v>
@@ -7239,8 +7278,12 @@
       <c r="M58" s="11"/>
       <c r="N58" s="11"/>
       <c r="O58" s="14"/>
-      <c r="P58" s="9"/>
-      <c r="Q58" s="11"/>
+      <c r="P58" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q58" s="53" t="s">
+        <v>114</v>
+      </c>
       <c r="R58" s="12"/>
       <c r="S58" s="11"/>
       <c r="T58" s="11"/>
@@ -7271,10 +7314,10 @@
       <c r="AO58" s="11"/>
       <c r="AP58" s="14"/>
       <c r="AQ58" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="AR58" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="AR58" s="11" t="s">
-        <v>268</v>
       </c>
       <c r="AS58" s="12"/>
       <c r="AT58" s="11"/>
@@ -7394,14 +7437,14 @@
       <c r="D60" s="9"/>
       <c r="E60" s="11"/>
       <c r="F60" s="12"/>
-      <c r="G60" s="36" t="s">
+      <c r="G60" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="34"/>
-      <c r="L60" s="35"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
+      <c r="K60" s="38"/>
+      <c r="L60" s="39"/>
       <c r="M60" s="11"/>
       <c r="N60" s="11"/>
       <c r="O60" s="14"/>
@@ -7427,7 +7470,7 @@
       <c r="AI60" s="11"/>
       <c r="AJ60" s="12"/>
       <c r="AK60" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AL60" s="11" t="s">
         <v>160</v>
@@ -7445,8 +7488,12 @@
       <c r="AW60" s="11"/>
       <c r="AX60" s="11"/>
       <c r="AY60" s="14"/>
-      <c r="AZ60" s="11"/>
-      <c r="BA60" s="11"/>
+      <c r="AZ60" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="BA60" s="57" t="s">
+        <v>114</v>
+      </c>
       <c r="BB60" s="13"/>
       <c r="BC60" s="11"/>
       <c r="BD60" s="11"/>
@@ -7472,14 +7519,14 @@
       <c r="C61" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G61" s="36" t="s">
+      <c r="G61" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="34"/>
-      <c r="L61" s="35"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="38"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="39"/>
       <c r="M61" s="11"/>
       <c r="N61" s="11"/>
       <c r="O61" s="14"/>
@@ -7516,14 +7563,14 @@
       <c r="AF61" s="11"/>
       <c r="AG61" s="14"/>
       <c r="AH61" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AI61" s="11" t="s">
         <v>121</v>
       </c>
       <c r="AJ61" s="12"/>
       <c r="AK61" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AL61" s="11" t="s">
         <v>191</v>
@@ -7543,10 +7590,10 @@
       </c>
       <c r="AX61" s="11"/>
       <c r="AY61" s="14"/>
-      <c r="AZ61" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="BA61" s="10" t="s">
+      <c r="AZ61" s="53" t="s">
+        <v>259</v>
+      </c>
+      <c r="BA61" s="53" t="s">
         <v>114</v>
       </c>
       <c r="BB61" s="13"/>
@@ -7574,14 +7621,14 @@
       <c r="C62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="34"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="35"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="39"/>
       <c r="K62" s="11"/>
       <c r="L62" s="12"/>
       <c r="M62" s="11"/>
@@ -7629,7 +7676,7 @@
       <c r="AI62" s="11"/>
       <c r="AJ62" s="12"/>
       <c r="AK62" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AL62" s="11" t="s">
         <v>191</v>
@@ -7639,10 +7686,10 @@
       <c r="AO62" s="11"/>
       <c r="AP62" s="14"/>
       <c r="AQ62" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="AR62" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="AR62" s="11" t="s">
-        <v>268</v>
       </c>
       <c r="AS62" s="12"/>
       <c r="AT62" s="11"/>
@@ -7651,8 +7698,12 @@
       <c r="AW62" s="11"/>
       <c r="AX62" s="11"/>
       <c r="AY62" s="14"/>
-      <c r="AZ62" s="11"/>
-      <c r="BA62" s="11"/>
+      <c r="AZ62" s="53" t="s">
+        <v>260</v>
+      </c>
+      <c r="BA62" s="53" t="s">
+        <v>114</v>
+      </c>
       <c r="BB62" s="13"/>
       <c r="BC62" s="11"/>
       <c r="BD62" s="11"/>
@@ -7732,8 +7783,6 @@
       <c r="AW63" s="11"/>
       <c r="AX63" s="11"/>
       <c r="AY63" s="14"/>
-      <c r="AZ63" s="11"/>
-      <c r="BA63" s="11"/>
       <c r="BB63" s="13"/>
       <c r="BC63" s="11"/>
       <c r="BD63" s="11"/>
@@ -7855,12 +7904,8 @@
       <c r="P65" s="9"/>
       <c r="Q65" s="11"/>
       <c r="R65" s="12"/>
-      <c r="S65" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="T65" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="S65" s="33"/>
+      <c r="T65" s="33"/>
       <c r="U65" s="12"/>
       <c r="V65" s="11"/>
       <c r="W65" s="11"/>
@@ -7886,7 +7931,7 @@
       <c r="AI65" s="11"/>
       <c r="AJ65" s="12"/>
       <c r="AK65" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AL65" s="11" t="s">
         <v>191</v>
@@ -7937,12 +7982,12 @@
         <v>107</v>
       </c>
       <c r="F66" s="12"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="34"/>
-      <c r="I66" s="34"/>
-      <c r="J66" s="34"/>
-      <c r="K66" s="34"/>
-      <c r="L66" s="35"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="38"/>
+      <c r="K66" s="38"/>
+      <c r="L66" s="39"/>
       <c r="M66" s="11" t="s">
         <v>104</v>
       </c>
@@ -7971,12 +8016,6 @@
         <v>158</v>
       </c>
       <c r="X66" s="14"/>
-      <c r="Y66" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="Z66" s="11" t="s">
-        <v>114</v>
-      </c>
       <c r="AA66" s="11"/>
       <c r="AB66" s="11" t="s">
         <v>189</v>
@@ -7993,14 +8032,14 @@
       </c>
       <c r="AG66" s="14"/>
       <c r="AH66" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AI66" s="11" t="s">
         <v>195</v>
       </c>
       <c r="AJ66" s="12"/>
       <c r="AK66" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AL66" s="11" t="s">
         <v>183</v>
@@ -8010,10 +8049,10 @@
       <c r="AO66" s="11"/>
       <c r="AP66" s="14"/>
       <c r="AQ66" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AR66" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AS66" s="12"/>
       <c r="AT66" s="11"/>
@@ -8056,21 +8095,17 @@
         <v>107</v>
       </c>
       <c r="F67" s="12"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="34"/>
-      <c r="J67" s="34"/>
-      <c r="K67" s="34"/>
-      <c r="L67" s="35"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
+      <c r="K67" s="38"/>
+      <c r="L67" s="39"/>
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q67" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="P67" s="56"/>
+      <c r="Q67" s="33"/>
       <c r="R67" s="12"/>
       <c r="U67" s="12"/>
       <c r="V67" s="11" t="s">
@@ -8091,7 +8126,7 @@
       <c r="AI67" s="11"/>
       <c r="AJ67" s="12"/>
       <c r="AK67" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AL67" s="11" t="s">
         <v>183</v>
@@ -8101,14 +8136,14 @@
       <c r="AO67" s="11"/>
       <c r="AP67" s="14"/>
       <c r="AQ67" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AR67" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AS67" s="12"/>
       <c r="AT67" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AU67" s="11" t="s">
         <v>137</v>
@@ -8334,7 +8369,7 @@
       <c r="AR70" s="11"/>
       <c r="AS70" s="12"/>
       <c r="AT70" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AU70" s="11" t="s">
         <v>137</v>
@@ -8370,14 +8405,14 @@
       <c r="C71" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D71" s="33" t="s">
+      <c r="D71" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="35"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="39"/>
       <c r="J71" s="11"/>
       <c r="K71" s="11"/>
       <c r="L71" s="12"/>
@@ -8424,24 +8459,24 @@
       <c r="AG71" s="14"/>
       <c r="AJ71" s="12"/>
       <c r="AK71" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AL71" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AM71" s="12"/>
       <c r="AN71" s="11"/>
       <c r="AO71" s="11"/>
       <c r="AP71" s="14"/>
       <c r="AQ71" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AR71" s="11" t="s">
         <v>173</v>
       </c>
       <c r="AS71" s="12"/>
       <c r="AT71" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AU71" s="11" t="s">
         <v>137</v>
@@ -8477,12 +8512,12 @@
       <c r="C72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D72" s="30"/>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="32"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="36"/>
       <c r="J72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="12"/>
@@ -8532,7 +8567,7 @@
       </c>
       <c r="AG72" s="14"/>
       <c r="AH72" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AI72" s="11" t="s">
         <v>173</v>
@@ -8559,14 +8594,14 @@
       <c r="BC72" s="11"/>
       <c r="BD72" s="11"/>
       <c r="BE72" s="12"/>
-      <c r="BF72" s="36" t="s">
-        <v>245</v>
-      </c>
-      <c r="BG72" s="34"/>
-      <c r="BH72" s="34"/>
-      <c r="BI72" s="34"/>
-      <c r="BJ72" s="34"/>
-      <c r="BK72" s="35"/>
+      <c r="BF72" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="BG72" s="38"/>
+      <c r="BH72" s="38"/>
+      <c r="BI72" s="38"/>
+      <c r="BJ72" s="38"/>
+      <c r="BK72" s="39"/>
       <c r="BL72" s="11"/>
       <c r="BM72" s="11"/>
       <c r="BN72" s="11"/>
@@ -8582,12 +8617,12 @@
       <c r="C73" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D73" s="30"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="32"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="35"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="35"/>
+      <c r="I73" s="36"/>
       <c r="J73" s="11"/>
       <c r="K73" s="11"/>
       <c r="L73" s="12"/>
@@ -8730,12 +8765,12 @@
       <c r="C75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="30"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="31"/>
-      <c r="H75" s="31"/>
-      <c r="I75" s="32"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="35"/>
+      <c r="H75" s="35"/>
+      <c r="I75" s="36"/>
       <c r="J75" s="11"/>
       <c r="K75" s="11"/>
       <c r="L75" s="12"/>
@@ -8813,14 +8848,14 @@
       <c r="C76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="30" t="s">
+      <c r="D76" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E76" s="31"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="31"/>
-      <c r="I76" s="31"/>
+      <c r="E76" s="35"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="35"/>
+      <c r="H76" s="35"/>
+      <c r="I76" s="35"/>
       <c r="J76" s="11"/>
       <c r="K76" s="11"/>
       <c r="L76" s="12"/>
@@ -8859,7 +8894,7 @@
       <c r="AI76" s="11"/>
       <c r="AJ76" s="12"/>
       <c r="AK76" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL76" s="11" t="s">
         <v>195</v>
@@ -8904,14 +8939,14 @@
       <c r="C77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D77" s="30" t="s">
+      <c r="D77" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E77" s="31"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-      <c r="H77" s="31"/>
-      <c r="I77" s="31"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="35"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11"/>
       <c r="L77" s="12"/>
@@ -8949,7 +8984,7 @@
       <c r="AF77" s="11"/>
       <c r="AG77" s="14"/>
       <c r="AH77" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AI77" s="11" t="s">
         <v>171</v>
@@ -8997,14 +9032,14 @@
       <c r="C78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="33" t="s">
+      <c r="D78" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="E78" s="34"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="34"/>
-      <c r="H78" s="34"/>
-      <c r="I78" s="35"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="39"/>
       <c r="J78" s="11"/>
       <c r="K78" s="11"/>
       <c r="L78" s="12"/>
@@ -9146,14 +9181,14 @@
       <c r="C80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="30" t="s">
+      <c r="D80" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E80" s="31"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
-      <c r="H80" s="31"/>
-      <c r="I80" s="31"/>
+      <c r="E80" s="35"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="35"/>
+      <c r="H80" s="35"/>
+      <c r="I80" s="35"/>
       <c r="J80" s="11"/>
       <c r="K80" s="11"/>
       <c r="L80" s="12"/>
@@ -9223,14 +9258,14 @@
       <c r="C81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="33" t="s">
+      <c r="D81" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="E81" s="34"/>
-      <c r="F81" s="34"/>
-      <c r="G81" s="34"/>
-      <c r="H81" s="34"/>
-      <c r="I81" s="35"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="38"/>
+      <c r="I81" s="39"/>
       <c r="J81" s="11"/>
       <c r="K81" s="11"/>
       <c r="L81" s="12"/>
@@ -9300,14 +9335,14 @@
       <c r="C82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D82" s="33" t="s">
+      <c r="D82" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="E82" s="34"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="34"/>
-      <c r="H82" s="34"/>
-      <c r="I82" s="35"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="38"/>
+      <c r="H82" s="38"/>
+      <c r="I82" s="39"/>
       <c r="J82" s="11"/>
       <c r="K82" s="11"/>
       <c r="L82" s="12"/>
@@ -9377,12 +9412,12 @@
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="30"/>
-      <c r="E83" s="31"/>
-      <c r="F83" s="31"/>
-      <c r="G83" s="31"/>
-      <c r="H83" s="31"/>
-      <c r="I83" s="32"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="35"/>
+      <c r="H83" s="35"/>
+      <c r="I83" s="36"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11"/>
       <c r="L83" s="12"/>
@@ -9826,6 +9861,7 @@
     <mergeCell ref="AZ2:BE2"/>
     <mergeCell ref="BF2:BK2"/>
     <mergeCell ref="BL2:BQ2"/>
+    <mergeCell ref="BO3:BQ3"/>
     <mergeCell ref="AZ1:BQ1"/>
     <mergeCell ref="AZ3:BB3"/>
     <mergeCell ref="BU3:BW3"/>
@@ -9842,7 +9878,6 @@
     <mergeCell ref="BF3:BH3"/>
     <mergeCell ref="BI3:BK3"/>
     <mergeCell ref="BL3:BN3"/>
-    <mergeCell ref="BO3:BQ3"/>
     <mergeCell ref="BR3:BT3"/>
     <mergeCell ref="AK2:AM3"/>
     <mergeCell ref="AN2:AP3"/>
@@ -9854,6 +9889,8 @@
     <mergeCell ref="P1:X1"/>
     <mergeCell ref="Y1:AG1"/>
     <mergeCell ref="AH1:AP1"/>
+    <mergeCell ref="D45:I45"/>
+    <mergeCell ref="D48:I48"/>
     <mergeCell ref="AQ1:AY1"/>
     <mergeCell ref="P26:X26"/>
     <mergeCell ref="P27:X27"/>
@@ -9868,12 +9905,6 @@
     <mergeCell ref="D27:I27"/>
     <mergeCell ref="D8:O8"/>
     <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="D17:O17"/>
-    <mergeCell ref="D10:O10"/>
-    <mergeCell ref="G51:L51"/>
-    <mergeCell ref="G52:L52"/>
     <mergeCell ref="D42:I42"/>
     <mergeCell ref="D43:I43"/>
     <mergeCell ref="D12:I12"/>
@@ -9884,8 +9915,8 @@
     <mergeCell ref="D32:O32"/>
     <mergeCell ref="D36:I36"/>
     <mergeCell ref="D37:I37"/>
-    <mergeCell ref="D45:I45"/>
-    <mergeCell ref="D48:I48"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D16:O16"/>
     <mergeCell ref="D29:I29"/>
     <mergeCell ref="AZ21:BE21"/>
     <mergeCell ref="AZ50:BE50"/>
@@ -9896,18 +9927,19 @@
     <mergeCell ref="BF43:BK43"/>
     <mergeCell ref="AK31:AP31"/>
     <mergeCell ref="AK32:AP32"/>
-    <mergeCell ref="G66:L66"/>
-    <mergeCell ref="G67:L67"/>
-    <mergeCell ref="G60:L60"/>
+    <mergeCell ref="P47:X47"/>
+    <mergeCell ref="P48:X48"/>
+    <mergeCell ref="D46:I46"/>
+    <mergeCell ref="D47:I47"/>
+    <mergeCell ref="D17:O17"/>
+    <mergeCell ref="D10:O10"/>
     <mergeCell ref="G61:L61"/>
     <mergeCell ref="AK51:AP51"/>
-    <mergeCell ref="P47:X47"/>
-    <mergeCell ref="P48:X48"/>
     <mergeCell ref="D62:I62"/>
     <mergeCell ref="G54:L54"/>
     <mergeCell ref="G55:L55"/>
-    <mergeCell ref="D46:I46"/>
-    <mergeCell ref="D47:I47"/>
+    <mergeCell ref="G51:L51"/>
+    <mergeCell ref="G52:L52"/>
     <mergeCell ref="D83:I83"/>
     <mergeCell ref="D56:I56"/>
     <mergeCell ref="D57:I57"/>
@@ -9921,8 +9953,12 @@
     <mergeCell ref="D76:I76"/>
     <mergeCell ref="D72:I72"/>
     <mergeCell ref="D73:I73"/>
+    <mergeCell ref="G66:L66"/>
+    <mergeCell ref="G67:L67"/>
+    <mergeCell ref="G60:L60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished R V.O. subjects
</commit_message>
<xml_diff>
--- a/Rozklad_2zaizd.xlsx
+++ b/Rozklad_2zaizd.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="S29" authorId="0" shapeId="0">
+    <comment ref="S29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S30" authorId="0" shapeId="0">
+    <comment ref="S30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S59" authorId="0" shapeId="0">
+    <comment ref="S59" authorId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="274">
   <si>
     <t>І</t>
   </si>
@@ -904,12 +904,15 @@
   </si>
   <si>
     <t>Грунтознавство (залік)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1168,7 +1171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1293,16 +1296,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1311,20 +1308,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1335,19 +1335,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1410,7 +1428,7 @@
     </a:clrScheme>
     <a:fontScheme name="Офіс">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1445,7 +1463,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1622,7 +1640,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1633,10 +1651,10 @@
   <dimension ref="A1:BW90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AL27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P58" sqref="P58:Q58"/>
+      <selection pane="bottomRight" activeCell="BF36" sqref="BF36:BK37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,9 +1695,9 @@
     <col min="34" max="34" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14" style="10" customWidth="1"/>
     <col min="38" max="38" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5" style="10" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.85546875" style="10" customWidth="1"/>
     <col min="40" max="40" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="5" style="10" bestFit="1" customWidth="1"/>
@@ -1720,277 +1738,277 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="53" t="s">
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="53" t="s">
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="53" t="s">
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="55"/>
-      <c r="AQ1" s="53" t="s">
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AM1" s="53"/>
+      <c r="AN1" s="53"/>
+      <c r="AO1" s="53"/>
+      <c r="AP1" s="54"/>
+      <c r="AQ1" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="AR1" s="54"/>
-      <c r="AS1" s="54"/>
-      <c r="AT1" s="54"/>
-      <c r="AU1" s="54"/>
-      <c r="AV1" s="54"/>
-      <c r="AW1" s="54"/>
-      <c r="AX1" s="54"/>
-      <c r="AY1" s="55"/>
-      <c r="AZ1" s="53" t="s">
+      <c r="AR1" s="53"/>
+      <c r="AS1" s="53"/>
+      <c r="AT1" s="53"/>
+      <c r="AU1" s="53"/>
+      <c r="AV1" s="53"/>
+      <c r="AW1" s="53"/>
+      <c r="AX1" s="53"/>
+      <c r="AY1" s="54"/>
+      <c r="AZ1" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="BA1" s="54"/>
-      <c r="BB1" s="54"/>
-      <c r="BC1" s="54"/>
-      <c r="BD1" s="54"/>
-      <c r="BE1" s="54"/>
-      <c r="BF1" s="54"/>
-      <c r="BG1" s="54"/>
-      <c r="BH1" s="54"/>
-      <c r="BI1" s="54"/>
-      <c r="BJ1" s="54"/>
-      <c r="BK1" s="54"/>
-      <c r="BL1" s="54"/>
-      <c r="BM1" s="54"/>
-      <c r="BN1" s="54"/>
-      <c r="BO1" s="54"/>
-      <c r="BP1" s="54"/>
-      <c r="BQ1" s="55"/>
+      <c r="BA1" s="53"/>
+      <c r="BB1" s="53"/>
+      <c r="BC1" s="53"/>
+      <c r="BD1" s="53"/>
+      <c r="BE1" s="53"/>
+      <c r="BF1" s="53"/>
+      <c r="BG1" s="53"/>
+      <c r="BH1" s="53"/>
+      <c r="BI1" s="53"/>
+      <c r="BJ1" s="53"/>
+      <c r="BK1" s="53"/>
+      <c r="BL1" s="53"/>
+      <c r="BM1" s="53"/>
+      <c r="BN1" s="53"/>
+      <c r="BO1" s="53"/>
+      <c r="BP1" s="53"/>
+      <c r="BQ1" s="54"/>
     </row>
     <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="51" t="s">
+      <c r="E2" s="46"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="51" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="51" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="50" t="s">
+      <c r="N2" s="46"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="51" t="s">
+      <c r="Q2" s="46"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="51"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="51" t="s">
+      <c r="T2" s="46"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="51"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="50" t="s">
+      <c r="W2" s="46"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="51" t="s">
+      <c r="Z2" s="46"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="56"/>
-      <c r="AE2" s="51" t="s">
+      <c r="AC2" s="46"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="50" t="s">
+      <c r="AF2" s="46"/>
+      <c r="AG2" s="47"/>
+      <c r="AH2" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="56"/>
-      <c r="AK2" s="51" t="s">
+      <c r="AI2" s="46"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="51" t="s">
+      <c r="AL2" s="46"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="52"/>
-      <c r="AQ2" s="50" t="s">
+      <c r="AO2" s="46"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="56"/>
-      <c r="AT2" s="51" t="s">
+      <c r="AR2" s="46"/>
+      <c r="AS2" s="49"/>
+      <c r="AT2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="56"/>
-      <c r="AW2" s="51" t="s">
+      <c r="AU2" s="46"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="AX2" s="51"/>
-      <c r="AY2" s="52"/>
-      <c r="AZ2" s="50" t="s">
+      <c r="AX2" s="46"/>
+      <c r="AY2" s="47"/>
+      <c r="AZ2" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="BA2" s="51"/>
-      <c r="BB2" s="51"/>
-      <c r="BC2" s="51"/>
-      <c r="BD2" s="51"/>
-      <c r="BE2" s="56"/>
-      <c r="BF2" s="59" t="s">
+      <c r="BA2" s="46"/>
+      <c r="BB2" s="46"/>
+      <c r="BC2" s="46"/>
+      <c r="BD2" s="46"/>
+      <c r="BE2" s="49"/>
+      <c r="BF2" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="BG2" s="51"/>
-      <c r="BH2" s="51"/>
-      <c r="BI2" s="51"/>
-      <c r="BJ2" s="51"/>
-      <c r="BK2" s="56"/>
-      <c r="BL2" s="51" t="s">
+      <c r="BG2" s="46"/>
+      <c r="BH2" s="46"/>
+      <c r="BI2" s="46"/>
+      <c r="BJ2" s="46"/>
+      <c r="BK2" s="49"/>
+      <c r="BL2" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="BM2" s="51"/>
-      <c r="BN2" s="51"/>
-      <c r="BO2" s="51"/>
-      <c r="BP2" s="51"/>
-      <c r="BQ2" s="52"/>
+      <c r="BM2" s="46"/>
+      <c r="BN2" s="46"/>
+      <c r="BO2" s="46"/>
+      <c r="BP2" s="46"/>
+      <c r="BQ2" s="47"/>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="50"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="51"/>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="52"/>
-      <c r="AH3" s="50"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="56"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="51"/>
-      <c r="AO3" s="51"/>
-      <c r="AP3" s="52"/>
-      <c r="AQ3" s="50"/>
-      <c r="AR3" s="51"/>
-      <c r="AS3" s="56"/>
-      <c r="AT3" s="51"/>
-      <c r="AU3" s="51"/>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="51"/>
-      <c r="AX3" s="51"/>
-      <c r="AY3" s="52"/>
-      <c r="AZ3" s="50" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="46"/>
+      <c r="AF3" s="46"/>
+      <c r="AG3" s="47"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="46"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="46"/>
+      <c r="AL3" s="46"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="46"/>
+      <c r="AO3" s="46"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="48"/>
+      <c r="AR3" s="46"/>
+      <c r="AS3" s="49"/>
+      <c r="AT3" s="46"/>
+      <c r="AU3" s="46"/>
+      <c r="AV3" s="49"/>
+      <c r="AW3" s="46"/>
+      <c r="AX3" s="46"/>
+      <c r="AY3" s="47"/>
+      <c r="AZ3" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="BA3" s="51"/>
-      <c r="BB3" s="58"/>
-      <c r="BC3" s="51" t="s">
+      <c r="BA3" s="46"/>
+      <c r="BB3" s="55"/>
+      <c r="BC3" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="BD3" s="51"/>
-      <c r="BE3" s="56"/>
-      <c r="BF3" s="59" t="s">
+      <c r="BD3" s="46"/>
+      <c r="BE3" s="49"/>
+      <c r="BF3" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="BG3" s="51"/>
-      <c r="BH3" s="58"/>
-      <c r="BI3" s="51" t="s">
+      <c r="BG3" s="46"/>
+      <c r="BH3" s="55"/>
+      <c r="BI3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="BJ3" s="51"/>
-      <c r="BK3" s="56"/>
-      <c r="BL3" s="51"/>
-      <c r="BM3" s="51"/>
-      <c r="BN3" s="58"/>
-      <c r="BO3" s="51" t="s">
+      <c r="BJ3" s="46"/>
+      <c r="BK3" s="49"/>
+      <c r="BL3" s="46"/>
+      <c r="BM3" s="46"/>
+      <c r="BN3" s="55"/>
+      <c r="BO3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="BP3" s="51"/>
-      <c r="BQ3" s="52"/>
-      <c r="BR3" s="57"/>
-      <c r="BS3" s="57"/>
-      <c r="BT3" s="57"/>
-      <c r="BU3" s="57"/>
-      <c r="BV3" s="57"/>
-      <c r="BW3" s="57"/>
+      <c r="BP3" s="46"/>
+      <c r="BQ3" s="47"/>
+      <c r="BR3" s="56"/>
+      <c r="BS3" s="56"/>
+      <c r="BT3" s="56"/>
+      <c r="BU3" s="56"/>
+      <c r="BV3" s="56"/>
+      <c r="BW3" s="56"/>
     </row>
     <row r="4" spans="1:75" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2208,14 +2226,14 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="56"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="49"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="4" t="s">
@@ -2305,14 +2323,14 @@
       <c r="BC5" s="4"/>
       <c r="BD5" s="4"/>
       <c r="BE5" s="5"/>
-      <c r="BF5" s="59" t="s">
+      <c r="BF5" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="BG5" s="51"/>
-      <c r="BH5" s="51"/>
-      <c r="BI5" s="51"/>
-      <c r="BJ5" s="51"/>
-      <c r="BK5" s="56"/>
+      <c r="BG5" s="46"/>
+      <c r="BH5" s="46"/>
+      <c r="BI5" s="46"/>
+      <c r="BJ5" s="46"/>
+      <c r="BK5" s="49"/>
       <c r="BL5" s="11"/>
       <c r="BM5" s="11"/>
       <c r="BN5" s="13"/>
@@ -2328,14 +2346,14 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="56"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
@@ -2426,14 +2444,14 @@
       <c r="BC6" s="4"/>
       <c r="BD6" s="4"/>
       <c r="BE6" s="5"/>
-      <c r="BF6" s="59" t="s">
+      <c r="BF6" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="BG6" s="51"/>
-      <c r="BH6" s="51"/>
-      <c r="BI6" s="51"/>
-      <c r="BJ6" s="51"/>
-      <c r="BK6" s="56"/>
+      <c r="BG6" s="46"/>
+      <c r="BH6" s="46"/>
+      <c r="BI6" s="46"/>
+      <c r="BJ6" s="46"/>
+      <c r="BK6" s="49"/>
       <c r="BL6" s="11"/>
       <c r="BM6" s="11"/>
       <c r="BN6" s="13"/>
@@ -2449,14 +2467,14 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="56"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="5"/>
@@ -2560,20 +2578,20 @@
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="47"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="5"/>
@@ -2723,20 +2741,20 @@
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="49"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="60"/>
       <c r="P10" s="36" t="s">
         <v>113</v>
       </c>
@@ -2836,20 +2854,20 @@
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="49"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="60"/>
       <c r="P11" s="36" t="s">
         <v>113</v>
       </c>
@@ -2955,14 +2973,14 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="12"/>
@@ -3074,14 +3092,14 @@
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="47"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="12"/>
@@ -3350,20 +3368,20 @@
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="49"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="60"/>
       <c r="P16" s="9" t="s">
         <v>58</v>
       </c>
@@ -3471,20 +3489,20 @@
       <c r="C17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="49"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="44"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="60"/>
       <c r="P17" s="9" t="s">
         <v>58</v>
       </c>
@@ -3818,14 +3836,14 @@
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="47"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="12"/>
@@ -3910,14 +3928,14 @@
       <c r="AW21" s="11"/>
       <c r="AX21" s="11"/>
       <c r="AY21" s="14"/>
-      <c r="AZ21" s="45" t="s">
+      <c r="AZ21" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="BA21" s="46"/>
-      <c r="BB21" s="46"/>
-      <c r="BC21" s="46"/>
-      <c r="BD21" s="46"/>
-      <c r="BE21" s="47"/>
+      <c r="BA21" s="44"/>
+      <c r="BB21" s="44"/>
+      <c r="BC21" s="44"/>
+      <c r="BD21" s="44"/>
+      <c r="BE21" s="45"/>
       <c r="BF21" s="11"/>
       <c r="BG21" s="11"/>
       <c r="BH21" s="13"/>
@@ -3939,14 +3957,14 @@
       <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
       <c r="L22" s="12"/>
@@ -4206,20 +4224,20 @@
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="49"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="60"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="12"/>
@@ -4283,14 +4301,14 @@
       <c r="C26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="45" t="s">
+      <c r="D26" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="47"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="45"/>
       <c r="J26" s="11" t="s">
         <v>91</v>
       </c>
@@ -4305,17 +4323,17 @@
         <v>63</v>
       </c>
       <c r="O26" s="14"/>
-      <c r="P26" s="45" t="s">
+      <c r="P26" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="46"/>
-      <c r="T26" s="46"/>
-      <c r="U26" s="46"/>
-      <c r="V26" s="46"/>
-      <c r="W26" s="46"/>
-      <c r="X26" s="49"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="44"/>
+      <c r="X26" s="60"/>
       <c r="AA26" s="12"/>
       <c r="AB26" s="15" t="s">
         <v>67</v>
@@ -4392,14 +4410,14 @@
       <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="47"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="45"/>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
       <c r="L27" s="12"/>
@@ -4410,17 +4428,17 @@
         <v>63</v>
       </c>
       <c r="O27" s="14"/>
-      <c r="P27" s="45" t="s">
+      <c r="P27" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="46"/>
-      <c r="T27" s="46"/>
-      <c r="U27" s="46"/>
-      <c r="V27" s="46"/>
-      <c r="W27" s="46"/>
-      <c r="X27" s="49"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="44"/>
+      <c r="X27" s="60"/>
       <c r="Y27" s="36" t="s">
         <v>165</v>
       </c>
@@ -4579,14 +4597,14 @@
       <c r="BQ28" s="14"/>
     </row>
     <row r="29" spans="1:69" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="57" t="s">
         <v>271</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="44"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
       <c r="L29" s="12"/>
@@ -4741,20 +4759,20 @@
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="49"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="60"/>
       <c r="P31" s="9" t="s">
         <v>116</v>
       </c>
@@ -4804,14 +4822,14 @@
         <v>224</v>
       </c>
       <c r="AJ31" s="12"/>
-      <c r="AK31" s="48" t="s">
+      <c r="AK31" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="AL31" s="46"/>
-      <c r="AM31" s="46"/>
-      <c r="AN31" s="46"/>
-      <c r="AO31" s="46"/>
-      <c r="AP31" s="49"/>
+      <c r="AL31" s="44"/>
+      <c r="AM31" s="44"/>
+      <c r="AN31" s="44"/>
+      <c r="AO31" s="44"/>
+      <c r="AP31" s="60"/>
       <c r="AQ31" s="9" t="s">
         <v>262</v>
       </c>
@@ -4850,20 +4868,20 @@
       <c r="C32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="46"/>
-      <c r="N32" s="46"/>
-      <c r="O32" s="49"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="60"/>
       <c r="P32" s="9" t="s">
         <v>58</v>
       </c>
@@ -4901,14 +4919,14 @@
       <c r="AH32" s="9"/>
       <c r="AI32" s="11"/>
       <c r="AJ32" s="12"/>
-      <c r="AK32" s="48" t="s">
+      <c r="AK32" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="AL32" s="46"/>
-      <c r="AM32" s="46"/>
-      <c r="AN32" s="46"/>
-      <c r="AO32" s="46"/>
-      <c r="AP32" s="49"/>
+      <c r="AL32" s="44"/>
+      <c r="AM32" s="44"/>
+      <c r="AN32" s="44"/>
+      <c r="AO32" s="44"/>
+      <c r="AP32" s="60"/>
       <c r="AQ32" s="10" t="s">
         <v>102</v>
       </c>
@@ -5022,14 +5040,14 @@
       <c r="C34" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="47"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="45"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
       <c r="L34" s="12"/>
@@ -5142,13 +5160,13 @@
         <v>224</v>
       </c>
       <c r="AJ35" s="12"/>
-      <c r="AK35" s="10" t="s">
+      <c r="AK35" s="65" t="s">
         <v>241</v>
       </c>
-      <c r="AL35" s="10" t="s">
+      <c r="AL35" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="AM35" s="12"/>
+      <c r="AM35" s="64"/>
       <c r="AN35" s="11"/>
       <c r="AO35" s="11"/>
       <c r="AP35" s="14"/>
@@ -5192,14 +5210,14 @@
       <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="47"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="45"/>
       <c r="J36" s="11"/>
       <c r="K36" s="11"/>
       <c r="L36" s="12"/>
@@ -5210,17 +5228,17 @@
         <v>63</v>
       </c>
       <c r="O36" s="14"/>
-      <c r="P36" s="45" t="s">
+      <c r="P36" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="46"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="46"/>
-      <c r="V36" s="46"/>
-      <c r="W36" s="46"/>
-      <c r="X36" s="49"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="44"/>
+      <c r="X36" s="60"/>
       <c r="Y36" s="9" t="s">
         <v>79</v>
       </c>
@@ -5264,12 +5282,14 @@
       <c r="BC36" s="11"/>
       <c r="BD36" s="11"/>
       <c r="BE36" s="12"/>
-      <c r="BF36" s="11"/>
-      <c r="BG36" s="11"/>
-      <c r="BH36" s="13"/>
-      <c r="BI36" s="11"/>
-      <c r="BJ36" s="11"/>
-      <c r="BK36" s="12"/>
+      <c r="BF36" s="61" t="s">
+        <v>273</v>
+      </c>
+      <c r="BG36" s="62"/>
+      <c r="BH36" s="62"/>
+      <c r="BI36" s="62"/>
+      <c r="BJ36" s="62"/>
+      <c r="BK36" s="63"/>
       <c r="BL36" s="11"/>
       <c r="BM36" s="11"/>
       <c r="BN36" s="13"/>
@@ -5285,14 +5305,14 @@
       <c r="C37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="D37" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="47"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="45"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
       <c r="L37" s="12"/>
@@ -5365,12 +5385,14 @@
       <c r="BC37" s="11"/>
       <c r="BD37" s="11"/>
       <c r="BE37" s="12"/>
-      <c r="BF37" s="11"/>
-      <c r="BG37" s="11"/>
-      <c r="BH37" s="13"/>
-      <c r="BI37" s="11"/>
-      <c r="BJ37" s="11"/>
-      <c r="BK37" s="12"/>
+      <c r="BF37" s="61" t="s">
+        <v>245</v>
+      </c>
+      <c r="BG37" s="62"/>
+      <c r="BH37" s="62"/>
+      <c r="BI37" s="62"/>
+      <c r="BJ37" s="62"/>
+      <c r="BK37" s="63"/>
       <c r="BL37" s="11"/>
       <c r="BM37" s="11"/>
       <c r="BN37" s="13"/>
@@ -5547,20 +5569,20 @@
       <c r="C40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="50" t="s">
+      <c r="D40" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="52"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="47"/>
       <c r="P40" s="9" t="s">
         <v>124</v>
       </c>
@@ -5637,14 +5659,14 @@
       <c r="BC40" s="11"/>
       <c r="BD40" s="11"/>
       <c r="BE40" s="12"/>
-      <c r="BF40" s="59" t="s">
+      <c r="BF40" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="BG40" s="51"/>
-      <c r="BH40" s="51"/>
-      <c r="BI40" s="51"/>
-      <c r="BJ40" s="51"/>
-      <c r="BK40" s="56"/>
+      <c r="BG40" s="46"/>
+      <c r="BH40" s="46"/>
+      <c r="BI40" s="46"/>
+      <c r="BJ40" s="46"/>
+      <c r="BK40" s="49"/>
       <c r="BL40" s="11"/>
       <c r="BM40" s="11"/>
       <c r="BN40" s="13"/>
@@ -5660,20 +5682,20 @@
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="50" t="s">
+      <c r="D41" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="52"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="47"/>
       <c r="P41" s="9" t="s">
         <v>124</v>
       </c>
@@ -5770,14 +5792,14 @@
       <c r="C42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="45" t="s">
+      <c r="D42" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="47"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="45"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
       <c r="L42" s="12"/>
@@ -5864,14 +5886,6 @@
       <c r="BC42" s="11"/>
       <c r="BD42" s="11"/>
       <c r="BE42" s="12"/>
-      <c r="BF42" s="48" t="s">
-        <v>245</v>
-      </c>
-      <c r="BG42" s="46"/>
-      <c r="BH42" s="46"/>
-      <c r="BI42" s="46"/>
-      <c r="BJ42" s="46"/>
-      <c r="BK42" s="47"/>
       <c r="BL42" s="11"/>
       <c r="BM42" s="11"/>
       <c r="BN42" s="13"/>
@@ -5887,14 +5901,14 @@
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="45" t="s">
+      <c r="D43" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="47"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="45"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
       <c r="L43" s="12"/>
@@ -5971,14 +5985,6 @@
       <c r="BC43" s="11"/>
       <c r="BD43" s="11"/>
       <c r="BE43" s="12"/>
-      <c r="BF43" s="48" t="s">
-        <v>245</v>
-      </c>
-      <c r="BG43" s="46"/>
-      <c r="BH43" s="46"/>
-      <c r="BI43" s="46"/>
-      <c r="BJ43" s="46"/>
-      <c r="BK43" s="47"/>
       <c r="BL43" s="11"/>
       <c r="BM43" s="11"/>
       <c r="BN43" s="13"/>
@@ -6064,14 +6070,14 @@
       <c r="C45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="44"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="59"/>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
       <c r="L45" s="12"/>
@@ -6165,14 +6171,14 @@
       <c r="C46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="42" t="s">
+      <c r="D46" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="44"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="59"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
       <c r="L46" s="12"/>
@@ -6270,31 +6276,31 @@
       <c r="C47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D47" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="59"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
       <c r="L47" s="12"/>
       <c r="M47" s="11"/>
       <c r="N47" s="11"/>
       <c r="O47" s="14"/>
-      <c r="P47" s="45" t="s">
+      <c r="P47" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="Q47" s="46"/>
-      <c r="R47" s="46"/>
-      <c r="S47" s="46"/>
-      <c r="T47" s="46"/>
-      <c r="U47" s="46"/>
-      <c r="V47" s="46"/>
-      <c r="W47" s="46"/>
-      <c r="X47" s="49"/>
+      <c r="Q47" s="44"/>
+      <c r="R47" s="44"/>
+      <c r="S47" s="44"/>
+      <c r="T47" s="44"/>
+      <c r="U47" s="44"/>
+      <c r="V47" s="44"/>
+      <c r="W47" s="44"/>
+      <c r="X47" s="60"/>
       <c r="Y47" s="9"/>
       <c r="Z47" s="11"/>
       <c r="AA47" s="12"/>
@@ -6365,31 +6371,31 @@
       <c r="C48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D48" s="42" t="s">
+      <c r="D48" s="57" t="s">
         <v>213</v>
       </c>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="44"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="59"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
       <c r="L48" s="12"/>
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
       <c r="O48" s="14"/>
-      <c r="P48" s="45" t="s">
+      <c r="P48" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="46"/>
-      <c r="S48" s="46"/>
-      <c r="T48" s="46"/>
-      <c r="U48" s="46"/>
-      <c r="V48" s="46"/>
-      <c r="W48" s="46"/>
-      <c r="X48" s="49"/>
+      <c r="Q48" s="44"/>
+      <c r="R48" s="44"/>
+      <c r="S48" s="44"/>
+      <c r="T48" s="44"/>
+      <c r="U48" s="44"/>
+      <c r="V48" s="44"/>
+      <c r="W48" s="44"/>
+      <c r="X48" s="60"/>
       <c r="Y48" s="11"/>
       <c r="Z48" s="11"/>
       <c r="AA48" s="11"/>
@@ -6593,14 +6599,14 @@
       <c r="AW50" s="11"/>
       <c r="AX50" s="11"/>
       <c r="AY50" s="14"/>
-      <c r="AZ50" s="45" t="s">
+      <c r="AZ50" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="BA50" s="46"/>
-      <c r="BB50" s="46"/>
-      <c r="BC50" s="46"/>
-      <c r="BD50" s="46"/>
-      <c r="BE50" s="47"/>
+      <c r="BA50" s="44"/>
+      <c r="BB50" s="44"/>
+      <c r="BC50" s="44"/>
+      <c r="BD50" s="44"/>
+      <c r="BE50" s="45"/>
       <c r="BF50" s="11"/>
       <c r="BG50" s="11"/>
       <c r="BH50" s="13"/>
@@ -6625,14 +6631,14 @@
       <c r="D51" s="9"/>
       <c r="E51" s="11"/>
       <c r="F51" s="12"/>
-      <c r="G51" s="48" t="s">
+      <c r="G51" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="H51" s="46"/>
-      <c r="I51" s="46"/>
-      <c r="J51" s="46"/>
-      <c r="K51" s="46"/>
-      <c r="L51" s="47"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="44"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="45"/>
       <c r="M51" s="10" t="s">
         <v>89</v>
       </c>
@@ -6685,14 +6691,14 @@
       <c r="AH51" s="11"/>
       <c r="AI51" s="11"/>
       <c r="AJ51" s="12"/>
-      <c r="AK51" s="48" t="s">
+      <c r="AK51" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="AL51" s="46"/>
-      <c r="AM51" s="46"/>
-      <c r="AN51" s="46"/>
-      <c r="AO51" s="46"/>
-      <c r="AP51" s="49"/>
+      <c r="AL51" s="44"/>
+      <c r="AM51" s="44"/>
+      <c r="AN51" s="44"/>
+      <c r="AO51" s="44"/>
+      <c r="AP51" s="60"/>
       <c r="AQ51" s="11"/>
       <c r="AR51" s="11"/>
       <c r="AS51" s="12"/>
@@ -6726,14 +6732,14 @@
       <c r="D52" s="9"/>
       <c r="E52" s="11"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="48" t="s">
+      <c r="G52" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="47"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="45"/>
       <c r="M52" s="10" t="s">
         <v>89</v>
       </c>
@@ -6905,14 +6911,14 @@
       <c r="D54" s="9"/>
       <c r="E54" s="11"/>
       <c r="F54" s="12"/>
-      <c r="G54" s="48" t="s">
+      <c r="G54" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="H54" s="46"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="46"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="47"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="44"/>
+      <c r="K54" s="44"/>
+      <c r="L54" s="45"/>
       <c r="M54" s="11"/>
       <c r="N54" s="11"/>
       <c r="O54" s="14"/>
@@ -6984,14 +6990,14 @@
       <c r="D55" s="9"/>
       <c r="E55" s="11"/>
       <c r="F55" s="12"/>
-      <c r="G55" s="48" t="s">
+      <c r="G55" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="H55" s="46"/>
-      <c r="I55" s="46"/>
-      <c r="J55" s="46"/>
-      <c r="K55" s="46"/>
-      <c r="L55" s="47"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="44"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="45"/>
       <c r="M55" s="11"/>
       <c r="N55" s="11"/>
       <c r="O55" s="14"/>
@@ -7058,14 +7064,14 @@
       <c r="C56" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="42" t="s">
+      <c r="D56" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
       <c r="M56" s="11" t="s">
         <v>105</v>
       </c>
@@ -7168,14 +7174,14 @@
       <c r="C57" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D57" s="42" t="s">
+      <c r="D57" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="58"/>
       <c r="M57" s="11" t="s">
         <v>105</v>
       </c>
@@ -7289,7 +7295,7 @@
       <c r="M58" s="11"/>
       <c r="N58" s="11"/>
       <c r="O58" s="14"/>
-      <c r="P58" s="60"/>
+      <c r="P58" s="42"/>
       <c r="Q58" s="32"/>
       <c r="R58" s="12"/>
       <c r="S58" s="11"/>
@@ -7444,14 +7450,14 @@
       <c r="D60" s="9"/>
       <c r="E60" s="11"/>
       <c r="F60" s="12"/>
-      <c r="G60" s="48" t="s">
+      <c r="G60" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="H60" s="46"/>
-      <c r="I60" s="46"/>
-      <c r="J60" s="46"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="47"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="45"/>
       <c r="M60" s="11"/>
       <c r="N60" s="11"/>
       <c r="O60" s="14"/>
@@ -7526,14 +7532,14 @@
       <c r="C61" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G61" s="48" t="s">
+      <c r="G61" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="47"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="45"/>
       <c r="M61" s="11"/>
       <c r="N61" s="11"/>
       <c r="O61" s="14"/>
@@ -7628,14 +7634,14 @@
       <c r="C62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="45" t="s">
+      <c r="D62" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="46"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="47"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="45"/>
       <c r="K62" s="11"/>
       <c r="L62" s="12"/>
       <c r="M62" s="11"/>
@@ -7989,12 +7995,12 @@
         <v>107</v>
       </c>
       <c r="F66" s="12"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="46"/>
-      <c r="J66" s="46"/>
-      <c r="K66" s="46"/>
-      <c r="L66" s="47"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="44"/>
+      <c r="J66" s="44"/>
+      <c r="K66" s="44"/>
+      <c r="L66" s="45"/>
       <c r="M66" s="11" t="s">
         <v>104</v>
       </c>
@@ -8102,12 +8108,12 @@
         <v>107</v>
       </c>
       <c r="F67" s="12"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="46"/>
-      <c r="I67" s="46"/>
-      <c r="J67" s="46"/>
-      <c r="K67" s="46"/>
-      <c r="L67" s="47"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="44"/>
+      <c r="I67" s="44"/>
+      <c r="J67" s="44"/>
+      <c r="K67" s="44"/>
+      <c r="L67" s="45"/>
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
       <c r="O67" s="14"/>
@@ -8366,9 +8372,13 @@
       <c r="AH70" s="11"/>
       <c r="AI70" s="11"/>
       <c r="AJ70" s="12"/>
-      <c r="AK70" s="11"/>
-      <c r="AL70" s="11"/>
-      <c r="AM70" s="12"/>
+      <c r="AK70" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="AL70" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="AM70" s="64"/>
       <c r="AN70" s="11"/>
       <c r="AO70" s="11"/>
       <c r="AP70" s="14"/>
@@ -8412,14 +8422,14 @@
       <c r="C71" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D71" s="45" t="s">
+      <c r="D71" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="E71" s="46"/>
-      <c r="F71" s="46"/>
-      <c r="G71" s="46"/>
-      <c r="H71" s="46"/>
-      <c r="I71" s="47"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="44"/>
+      <c r="I71" s="45"/>
       <c r="J71" s="11"/>
       <c r="K71" s="11"/>
       <c r="L71" s="12"/>
@@ -8465,12 +8475,6 @@
       </c>
       <c r="AG71" s="14"/>
       <c r="AJ71" s="12"/>
-      <c r="AK71" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="AL71" s="11" t="s">
-        <v>242</v>
-      </c>
       <c r="AM71" s="12"/>
       <c r="AN71" s="11"/>
       <c r="AO71" s="11"/>
@@ -8498,12 +8502,14 @@
       <c r="BC71" s="11"/>
       <c r="BD71" s="11"/>
       <c r="BE71" s="12"/>
-      <c r="BF71" s="11"/>
-      <c r="BG71" s="11"/>
-      <c r="BH71" s="13"/>
-      <c r="BI71" s="11"/>
-      <c r="BJ71" s="11"/>
-      <c r="BK71" s="12"/>
+      <c r="BF71" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="BG71" s="62"/>
+      <c r="BH71" s="62"/>
+      <c r="BI71" s="62"/>
+      <c r="BJ71" s="62"/>
+      <c r="BK71" s="63"/>
       <c r="BL71" s="11"/>
       <c r="BM71" s="11"/>
       <c r="BN71" s="11"/>
@@ -8519,12 +8525,12 @@
       <c r="C72" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D72" s="42"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="43"/>
-      <c r="I72" s="44"/>
+      <c r="D72" s="57"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="59"/>
       <c r="J72" s="11"/>
       <c r="K72" s="11"/>
       <c r="L72" s="12"/>
@@ -8601,14 +8607,6 @@
       <c r="BC72" s="11"/>
       <c r="BD72" s="11"/>
       <c r="BE72" s="12"/>
-      <c r="BF72" s="48" t="s">
-        <v>244</v>
-      </c>
-      <c r="BG72" s="46"/>
-      <c r="BH72" s="46"/>
-      <c r="BI72" s="46"/>
-      <c r="BJ72" s="46"/>
-      <c r="BK72" s="47"/>
       <c r="BL72" s="11"/>
       <c r="BM72" s="11"/>
       <c r="BN72" s="11"/>
@@ -8624,12 +8622,12 @@
       <c r="C73" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D73" s="42"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="43"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="44"/>
+      <c r="D73" s="57"/>
+      <c r="E73" s="58"/>
+      <c r="F73" s="58"/>
+      <c r="G73" s="58"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="59"/>
       <c r="J73" s="11"/>
       <c r="K73" s="11"/>
       <c r="L73" s="12"/>
@@ -8772,12 +8770,12 @@
       <c r="C75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="42"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="43"/>
-      <c r="I75" s="44"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="58"/>
+      <c r="F75" s="58"/>
+      <c r="G75" s="58"/>
+      <c r="H75" s="58"/>
+      <c r="I75" s="59"/>
       <c r="J75" s="11"/>
       <c r="K75" s="11"/>
       <c r="L75" s="12"/>
@@ -8855,14 +8853,14 @@
       <c r="C76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="42" t="s">
+      <c r="D76" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="43"/>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
+      <c r="E76" s="58"/>
+      <c r="F76" s="58"/>
+      <c r="G76" s="58"/>
+      <c r="H76" s="58"/>
+      <c r="I76" s="58"/>
       <c r="J76" s="11"/>
       <c r="K76" s="11"/>
       <c r="L76" s="12"/>
@@ -8946,14 +8944,14 @@
       <c r="C77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D77" s="42" t="s">
+      <c r="D77" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="43"/>
-      <c r="H77" s="43"/>
-      <c r="I77" s="43"/>
+      <c r="E77" s="58"/>
+      <c r="F77" s="58"/>
+      <c r="G77" s="58"/>
+      <c r="H77" s="58"/>
+      <c r="I77" s="58"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11"/>
       <c r="L77" s="12"/>
@@ -9039,14 +9037,14 @@
       <c r="C78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="45" t="s">
+      <c r="D78" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="E78" s="46"/>
-      <c r="F78" s="46"/>
-      <c r="G78" s="46"/>
-      <c r="H78" s="46"/>
-      <c r="I78" s="47"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="44"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="44"/>
+      <c r="I78" s="45"/>
       <c r="J78" s="11"/>
       <c r="K78" s="11"/>
       <c r="L78" s="12"/>
@@ -9188,14 +9186,14 @@
       <c r="C80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="42" t="s">
+      <c r="D80" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="43"/>
-      <c r="H80" s="43"/>
-      <c r="I80" s="43"/>
+      <c r="E80" s="58"/>
+      <c r="F80" s="58"/>
+      <c r="G80" s="58"/>
+      <c r="H80" s="58"/>
+      <c r="I80" s="58"/>
       <c r="J80" s="11"/>
       <c r="K80" s="11"/>
       <c r="L80" s="12"/>
@@ -9265,14 +9263,14 @@
       <c r="C81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="45" t="s">
+      <c r="D81" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="E81" s="46"/>
-      <c r="F81" s="46"/>
-      <c r="G81" s="46"/>
-      <c r="H81" s="46"/>
-      <c r="I81" s="47"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="44"/>
+      <c r="I81" s="45"/>
       <c r="J81" s="11"/>
       <c r="K81" s="11"/>
       <c r="L81" s="12"/>
@@ -9342,14 +9340,14 @@
       <c r="C82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D82" s="45" t="s">
+      <c r="D82" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="46"/>
-      <c r="H82" s="46"/>
-      <c r="I82" s="47"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="44"/>
+      <c r="H82" s="44"/>
+      <c r="I82" s="45"/>
       <c r="J82" s="11"/>
       <c r="K82" s="11"/>
       <c r="L82" s="12"/>
@@ -9419,12 +9417,12 @@
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="42"/>
-      <c r="E83" s="43"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="43"/>
-      <c r="H83" s="43"/>
-      <c r="I83" s="44"/>
+      <c r="D83" s="57"/>
+      <c r="E83" s="58"/>
+      <c r="F83" s="58"/>
+      <c r="G83" s="58"/>
+      <c r="H83" s="58"/>
+      <c r="I83" s="59"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11"/>
       <c r="L83" s="12"/>
@@ -9863,19 +9861,77 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="BF72:BK72"/>
-    <mergeCell ref="AW2:AY3"/>
-    <mergeCell ref="AZ2:BE2"/>
-    <mergeCell ref="BF2:BK2"/>
-    <mergeCell ref="BL2:BQ2"/>
-    <mergeCell ref="BO3:BQ3"/>
-    <mergeCell ref="AZ21:BE21"/>
-    <mergeCell ref="AZ50:BE50"/>
-    <mergeCell ref="BF5:BK5"/>
-    <mergeCell ref="BF6:BK6"/>
-    <mergeCell ref="BF40:BK40"/>
-    <mergeCell ref="BF42:BK42"/>
-    <mergeCell ref="BF43:BK43"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="D56:I56"/>
+    <mergeCell ref="D57:I57"/>
+    <mergeCell ref="D77:I77"/>
+    <mergeCell ref="D71:I71"/>
+    <mergeCell ref="D78:I78"/>
+    <mergeCell ref="D80:I80"/>
+    <mergeCell ref="D81:I81"/>
+    <mergeCell ref="D82:I82"/>
+    <mergeCell ref="D75:I75"/>
+    <mergeCell ref="D76:I76"/>
+    <mergeCell ref="D72:I72"/>
+    <mergeCell ref="D73:I73"/>
+    <mergeCell ref="G66:L66"/>
+    <mergeCell ref="G67:L67"/>
+    <mergeCell ref="G60:L60"/>
+    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="AK51:AP51"/>
+    <mergeCell ref="D62:I62"/>
+    <mergeCell ref="G54:L54"/>
+    <mergeCell ref="G55:L55"/>
+    <mergeCell ref="G51:L51"/>
+    <mergeCell ref="G52:L52"/>
+    <mergeCell ref="AK31:AP31"/>
+    <mergeCell ref="AK32:AP32"/>
+    <mergeCell ref="P47:X47"/>
+    <mergeCell ref="P48:X48"/>
+    <mergeCell ref="D46:I46"/>
+    <mergeCell ref="D47:I47"/>
+    <mergeCell ref="D42:I42"/>
+    <mergeCell ref="D43:I43"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D41:O41"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="D32:O32"/>
+    <mergeCell ref="D36:I36"/>
+    <mergeCell ref="D37:I37"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D16:O16"/>
+    <mergeCell ref="D29:I29"/>
+    <mergeCell ref="D17:O17"/>
+    <mergeCell ref="D45:I45"/>
+    <mergeCell ref="D48:I48"/>
+    <mergeCell ref="AQ1:AY1"/>
+    <mergeCell ref="P26:X26"/>
+    <mergeCell ref="P27:X27"/>
+    <mergeCell ref="P36:X36"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D27:I27"/>
+    <mergeCell ref="D8:O8"/>
+    <mergeCell ref="D11:O11"/>
+    <mergeCell ref="AE2:AG3"/>
+    <mergeCell ref="AH2:AJ3"/>
+    <mergeCell ref="D1:O1"/>
+    <mergeCell ref="P1:X1"/>
+    <mergeCell ref="Y1:AG1"/>
+    <mergeCell ref="AH1:AP1"/>
+    <mergeCell ref="BR3:BT3"/>
+    <mergeCell ref="AK2:AM3"/>
+    <mergeCell ref="AN2:AP3"/>
+    <mergeCell ref="AQ2:AS3"/>
+    <mergeCell ref="AT2:AV3"/>
     <mergeCell ref="AZ1:BQ1"/>
     <mergeCell ref="AZ3:BB3"/>
     <mergeCell ref="BU3:BW3"/>
@@ -9892,77 +9948,19 @@
     <mergeCell ref="BF3:BH3"/>
     <mergeCell ref="BI3:BK3"/>
     <mergeCell ref="BL3:BN3"/>
-    <mergeCell ref="BR3:BT3"/>
-    <mergeCell ref="AK2:AM3"/>
-    <mergeCell ref="AN2:AP3"/>
-    <mergeCell ref="AQ2:AS3"/>
-    <mergeCell ref="AT2:AV3"/>
-    <mergeCell ref="AE2:AG3"/>
-    <mergeCell ref="AH2:AJ3"/>
-    <mergeCell ref="D1:O1"/>
-    <mergeCell ref="P1:X1"/>
-    <mergeCell ref="Y1:AG1"/>
-    <mergeCell ref="AH1:AP1"/>
-    <mergeCell ref="D45:I45"/>
-    <mergeCell ref="D48:I48"/>
-    <mergeCell ref="AQ1:AY1"/>
-    <mergeCell ref="P26:X26"/>
-    <mergeCell ref="P27:X27"/>
-    <mergeCell ref="P36:X36"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D34:I34"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="D27:I27"/>
-    <mergeCell ref="D8:O8"/>
-    <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="D40:O40"/>
-    <mergeCell ref="D41:O41"/>
-    <mergeCell ref="D31:O31"/>
-    <mergeCell ref="D32:O32"/>
-    <mergeCell ref="D36:I36"/>
-    <mergeCell ref="D37:I37"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="D29:I29"/>
-    <mergeCell ref="D17:O17"/>
-    <mergeCell ref="D10:O10"/>
-    <mergeCell ref="G61:L61"/>
-    <mergeCell ref="AK51:AP51"/>
-    <mergeCell ref="D62:I62"/>
-    <mergeCell ref="G54:L54"/>
-    <mergeCell ref="G55:L55"/>
-    <mergeCell ref="G51:L51"/>
-    <mergeCell ref="G52:L52"/>
-    <mergeCell ref="AK31:AP31"/>
-    <mergeCell ref="AK32:AP32"/>
-    <mergeCell ref="P47:X47"/>
-    <mergeCell ref="P48:X48"/>
-    <mergeCell ref="D46:I46"/>
-    <mergeCell ref="D47:I47"/>
-    <mergeCell ref="D42:I42"/>
-    <mergeCell ref="D43:I43"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="D56:I56"/>
-    <mergeCell ref="D57:I57"/>
-    <mergeCell ref="D77:I77"/>
-    <mergeCell ref="D71:I71"/>
-    <mergeCell ref="D78:I78"/>
-    <mergeCell ref="D80:I80"/>
-    <mergeCell ref="D81:I81"/>
-    <mergeCell ref="D82:I82"/>
-    <mergeCell ref="D75:I75"/>
-    <mergeCell ref="D76:I76"/>
-    <mergeCell ref="D72:I72"/>
-    <mergeCell ref="D73:I73"/>
-    <mergeCell ref="G66:L66"/>
-    <mergeCell ref="G67:L67"/>
-    <mergeCell ref="G60:L60"/>
+    <mergeCell ref="BF71:BK71"/>
+    <mergeCell ref="AW2:AY3"/>
+    <mergeCell ref="AZ2:BE2"/>
+    <mergeCell ref="BF2:BK2"/>
+    <mergeCell ref="BL2:BQ2"/>
+    <mergeCell ref="BO3:BQ3"/>
+    <mergeCell ref="AZ21:BE21"/>
+    <mergeCell ref="AZ50:BE50"/>
+    <mergeCell ref="BF5:BK5"/>
+    <mergeCell ref="BF6:BK6"/>
+    <mergeCell ref="BF40:BK40"/>
+    <mergeCell ref="BF36:BK36"/>
+    <mergeCell ref="BF37:BK37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>